<commit_message>
Added description for civ
</commit_message>
<xml_diff>
--- a/src/main/resources/assets/gamedata-faf-waw.xlsx
+++ b/src/main/resources/assets/gamedata-faf-waw.xlsx
@@ -5,7 +5,7 @@
   <workbookPr backupFile="false" showObjects="all" date1904="false"/>
   <workbookProtection/>
   <bookViews>
-    <workbookView showHorizontalScroll="true" showVerticalScroll="true" showSheetTabs="true" xWindow="0" yWindow="0" windowWidth="16384" windowHeight="8192" tabRatio="600" firstSheet="0" activeTab="4"/>
+    <workbookView showHorizontalScroll="true" showVerticalScroll="true" showSheetTabs="true" xWindow="0" yWindow="0" windowWidth="16384" windowHeight="8192" tabRatio="600" firstSheet="0" activeTab="0"/>
   </bookViews>
   <sheets>
     <sheet name="Civ" sheetId="1" state="visible" r:id="rId2"/>
@@ -32,7 +32,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="531" uniqueCount="352">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="548" uniqueCount="368">
   <si>
     <t>Civilization</t>
   </si>
@@ -40,106 +40,154 @@
     <t>Starting Tech</t>
   </si>
   <si>
+    <t>Description</t>
+  </si>
+  <si>
     <t>Americans</t>
   </si>
   <si>
     <t>Currency</t>
   </si>
   <si>
+    <t>The Americans start with a free random great person in their capital. Each time the Americans convert 3 trade into production, they receive 2 production instead of 1.</t>
+  </si>
+  <si>
     <t>Arabs</t>
   </si>
   <si>
     <t>Mathematics</t>
   </si>
   <si>
+    <t>The Arabs start the game with one of each resource from the market. For each resource token the Arabs spend for any reason, they gain 1 culture. Each time the Arabs invest a coin, they advance once space up the culture track for free</t>
+  </si>
+  <si>
     <t>Aztecs</t>
   </si>
   <si>
     <t>Irrigation</t>
   </si>
   <si>
+    <t>Each time the Aztecs win a battle, they gain 3 trade. After the Aztecs fight a battle, they gain 1 culture for each unit that was killed in the battle. Each time the Aztecs gain a great person, they may build 2 unlocked units of their choice for free.</t>
+  </si>
+  <si>
     <t>Chinese</t>
   </si>
   <si>
     <t>Writing</t>
   </si>
   <si>
+    <t>The Chinese start with city walls in their capital. The Chinese gain 3 culture each time they explore a hut or conquer a village. The Chinese may save one of their killed unit after each battle, returning it to their standing force</t>
+  </si>
+  <si>
     <t>Egyptians</t>
   </si>
   <si>
     <t>Construction</t>
   </si>
   <si>
+    <t>The Egyptians start with a free random ancient wonder in their capital. Once per turn, during City Management, the Egyptians may build an unlocked building for free by using an action.</t>
+  </si>
+  <si>
     <t>England</t>
   </si>
   <si>
     <t>Navy</t>
   </si>
   <si>
+    <t>English armies may gather icons and resources as though they where scouts. English figures may cross water, but may not end their movement in it.</t>
+  </si>
+  <si>
     <t>French</t>
   </si>
   <si>
     <t>Pottery</t>
   </si>
   <si>
+    <t>France start with +2 in combat bonus. The maximum number of social policies the French can adopt is increased by 1. The French starts with 1 extra social policy.</t>
+  </si>
+  <si>
     <t>Germans</t>
   </si>
   <si>
     <t>Metalworking</t>
   </si>
   <si>
+    <t>The Germans start with 2 extra infantry units. After setup, each time the Germans research a tech that upgrades or unlocked a unit, they build one of that unit for free and gain one resource of their choice from the market.</t>
+  </si>
+  <si>
     <t>Greeks</t>
   </si>
   <si>
     <t>Democracy</t>
   </si>
   <si>
+    <t>Each time the Greeks gain a great person, they draw one extra great person, keeping one and discarding the other.</t>
+  </si>
+  <si>
     <t>Indians</t>
   </si>
   <si>
     <t>Agriculture</t>
   </si>
   <si>
+    <t>The Indians start with a metropolis as their capital. When the Indians spend a resource, they may use it as incense, silk, iron or wheat. When the Indians devote a city to the arts, it produces 1 extra culture for each square containing a resource (silk, iron etc) in its outskirts.</t>
+  </si>
+  <si>
     <t>Japanese</t>
   </si>
   <si>
     <t>Chivalry</t>
   </si>
   <si>
+    <t>Japanese infantry units have +1 in strength. The Japanese require 3 less trade to research new techs of any level. </t>
+  </si>
+  <si>
     <t>Mongols</t>
   </si>
   <si>
     <t>Horseback Riding</t>
   </si>
   <si>
+    <t>The Mongols start with 2 extra mounted units. When attacking, if the Mongols gain loot, they gain 1 extra loot.</t>
+  </si>
+  <si>
     <t>Romans</t>
   </si>
   <si>
     <t>Code of Laws</t>
   </si>
   <si>
+    <t>The Romans advance one space on the culture track for free each time they build a wonder or city, and each time they conquer a city or village.</t>
+  </si>
+  <si>
     <t>Russians</t>
   </si>
   <si>
     <t>Communism</t>
   </si>
   <si>
+    <t>The Russians start with 2 extra armies, and their stacking limit is increased by 1. Once per turn, the Russians maybe move an army or scout into an enemy city and sacrifice that figure to research a tech known by that civilization for free. Armies sacrificed this way cannot be also attack.</t>
+  </si>
+  <si>
     <t>Spanish</t>
   </si>
   <si>
     <t>Navigation</t>
   </si>
   <si>
+    <t>The Spanish start with 2 scouts. The travel speed of the Spanish is increased by 1. When the Spanish discover an unexplored map tile, they may immediately build a basic (non-upgraded) building in any of their cities for free, even if they haven't unlocked that building.</t>
+  </si>
+  <si>
     <t>Zulu</t>
   </si>
   <si>
     <t>Animal Husbandry</t>
   </si>
   <si>
+    <t>The Zulu start with 2 extra artillery units. Zulu armies explore barbarian villages without a battle. The Zulu may build cities adjacent to huts, if they do, they may immediately explore those huts.</t>
+  </si>
+  <si>
     <t>Card Name</t>
-  </si>
-  <si>
-    <t>Description</t>
   </si>
   <si>
     <t>A Gift from Afar</t>
@@ -1224,16 +1272,17 @@
   <sheetPr filterMode="false">
     <pageSetUpPr fitToPage="false"/>
   </sheetPr>
-  <dimension ref="A1:B17"/>
+  <dimension ref="A1:C17"/>
   <sheetViews>
-    <sheetView windowProtection="false" showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="B1" activeCellId="0" sqref="B1"/>
+    <sheetView windowProtection="false" showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
+      <selection pane="topLeft" activeCell="C17" activeCellId="0" sqref="C17"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15"/>
   <cols>
     <col collapsed="false" hidden="false" max="1" min="1" style="0" width="23.2793522267206"/>
-    <col collapsed="false" hidden="false" max="4" min="2" style="0" width="11.4251012145749"/>
+    <col collapsed="false" hidden="false" max="2" min="2" style="0" width="19.1821862348178"/>
+    <col collapsed="false" hidden="false" max="4" min="3" style="0" width="11.4251012145749"/>
     <col collapsed="false" hidden="false" max="1025" min="5" style="0" width="8.57085020242915"/>
   </cols>
   <sheetData>
@@ -1244,133 +1293,184 @@
       <c r="B1" s="1" t="s">
         <v>1</v>
       </c>
+      <c r="C1" s="1" t="s">
+        <v>2</v>
+      </c>
     </row>
     <row r="2" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A2" s="0" t="s">
-        <v>2</v>
+        <v>3</v>
       </c>
       <c r="B2" s="0" t="s">
-        <v>3</v>
+        <v>4</v>
+      </c>
+      <c r="C2" s="0" t="s">
+        <v>5</v>
       </c>
     </row>
     <row r="3" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A3" s="0" t="s">
-        <v>4</v>
+        <v>6</v>
       </c>
       <c r="B3" s="0" t="s">
-        <v>5</v>
+        <v>7</v>
+      </c>
+      <c r="C3" s="0" t="s">
+        <v>8</v>
       </c>
     </row>
     <row r="4" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A4" s="0" t="s">
-        <v>6</v>
+        <v>9</v>
       </c>
       <c r="B4" s="0" t="s">
-        <v>7</v>
+        <v>10</v>
+      </c>
+      <c r="C4" s="0" t="s">
+        <v>11</v>
       </c>
     </row>
     <row r="5" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A5" s="2" t="s">
-        <v>8</v>
+        <v>12</v>
       </c>
       <c r="B5" s="0" t="s">
-        <v>9</v>
+        <v>13</v>
+      </c>
+      <c r="C5" s="0" t="s">
+        <v>14</v>
       </c>
     </row>
     <row r="6" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A6" s="2" t="s">
-        <v>10</v>
+        <v>15</v>
       </c>
       <c r="B6" s="0" t="s">
-        <v>11</v>
+        <v>16</v>
+      </c>
+      <c r="C6" s="0" t="s">
+        <v>17</v>
       </c>
     </row>
     <row r="7" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A7" s="0" t="s">
-        <v>12</v>
+        <v>18</v>
       </c>
       <c r="B7" s="0" t="s">
-        <v>13</v>
+        <v>19</v>
+      </c>
+      <c r="C7" s="0" t="s">
+        <v>20</v>
       </c>
     </row>
     <row r="8" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A8" s="0" t="s">
-        <v>14</v>
+        <v>21</v>
       </c>
       <c r="B8" s="0" t="s">
-        <v>15</v>
+        <v>22</v>
+      </c>
+      <c r="C8" s="0" t="s">
+        <v>23</v>
       </c>
     </row>
     <row r="9" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A9" s="0" t="s">
-        <v>16</v>
+        <v>24</v>
       </c>
       <c r="B9" s="0" t="s">
-        <v>17</v>
+        <v>25</v>
+      </c>
+      <c r="C9" s="0" t="s">
+        <v>26</v>
       </c>
     </row>
     <row r="10" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A10" s="0" t="s">
-        <v>18</v>
+        <v>27</v>
       </c>
       <c r="B10" s="0" t="s">
-        <v>19</v>
+        <v>28</v>
+      </c>
+      <c r="C10" s="0" t="s">
+        <v>29</v>
       </c>
     </row>
     <row r="11" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A11" s="0" t="s">
-        <v>20</v>
+        <v>30</v>
       </c>
       <c r="B11" s="0" t="s">
-        <v>21</v>
+        <v>31</v>
+      </c>
+      <c r="C11" s="0" t="s">
+        <v>32</v>
       </c>
     </row>
     <row r="12" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A12" s="0" t="s">
-        <v>22</v>
+        <v>33</v>
       </c>
       <c r="B12" s="0" t="s">
-        <v>23</v>
+        <v>34</v>
+      </c>
+      <c r="C12" s="0" t="s">
+        <v>35</v>
       </c>
     </row>
     <row r="13" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A13" s="0" t="s">
-        <v>24</v>
+        <v>36</v>
       </c>
       <c r="B13" s="0" t="s">
-        <v>25</v>
+        <v>37</v>
+      </c>
+      <c r="C13" s="0" t="s">
+        <v>38</v>
       </c>
     </row>
     <row r="14" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A14" s="2" t="s">
-        <v>26</v>
+        <v>39</v>
       </c>
       <c r="B14" s="0" t="s">
-        <v>27</v>
+        <v>40</v>
+      </c>
+      <c r="C14" s="0" t="s">
+        <v>41</v>
       </c>
     </row>
     <row r="15" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A15" s="2" t="s">
-        <v>28</v>
+        <v>42</v>
       </c>
       <c r="B15" s="0" t="s">
-        <v>29</v>
+        <v>43</v>
+      </c>
+      <c r="C15" s="0" t="s">
+        <v>44</v>
       </c>
     </row>
     <row r="16" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A16" s="0" t="s">
-        <v>30</v>
+        <v>45</v>
       </c>
       <c r="B16" s="0" t="s">
-        <v>31</v>
+        <v>46</v>
+      </c>
+      <c r="C16" s="0" t="s">
+        <v>47</v>
       </c>
     </row>
     <row r="17" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A17" s="0" t="s">
-        <v>32</v>
+        <v>48</v>
       </c>
       <c r="B17" s="0" t="s">
-        <v>33</v>
+        <v>49</v>
+      </c>
+      <c r="C17" s="0" t="s">
+        <v>50</v>
       </c>
     </row>
   </sheetData>
@@ -1403,108 +1503,108 @@
   <sheetData>
     <row r="1" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A1" s="1" t="s">
-        <v>215</v>
+        <v>231</v>
       </c>
       <c r="B1" s="1"/>
     </row>
     <row r="2" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A2" s="0" t="s">
-        <v>216</v>
+        <v>232</v>
       </c>
     </row>
     <row r="3" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A3" s="0" t="s">
-        <v>216</v>
+        <v>232</v>
       </c>
     </row>
     <row r="4" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A4" s="0" t="s">
-        <v>216</v>
+        <v>232</v>
       </c>
     </row>
     <row r="5" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A5" s="0" t="s">
-        <v>217</v>
+        <v>233</v>
       </c>
     </row>
     <row r="6" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A6" s="0" t="s">
-        <v>218</v>
+        <v>234</v>
       </c>
     </row>
     <row r="7" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A7" s="0" t="s">
-        <v>218</v>
+        <v>234</v>
       </c>
     </row>
     <row r="8" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A8" s="0" t="s">
-        <v>219</v>
+        <v>235</v>
       </c>
     </row>
     <row r="9" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A9" s="0" t="s">
-        <v>219</v>
+        <v>235</v>
       </c>
     </row>
     <row r="10" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A10" s="0" t="s">
-        <v>219</v>
+        <v>235</v>
       </c>
     </row>
     <row r="11" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A11" s="0" t="s">
-        <v>220</v>
+        <v>236</v>
       </c>
     </row>
     <row r="12" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A12" s="0" t="s">
-        <v>221</v>
+        <v>237</v>
       </c>
     </row>
     <row r="13" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A13" s="0" t="s">
-        <v>221</v>
+        <v>237</v>
       </c>
     </row>
     <row r="14" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A14" s="0" t="s">
-        <v>221</v>
+        <v>237</v>
       </c>
     </row>
     <row r="15" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A15" s="0" t="s">
-        <v>221</v>
+        <v>237</v>
       </c>
     </row>
     <row r="16" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A16" s="0" t="s">
-        <v>222</v>
+        <v>238</v>
       </c>
     </row>
     <row r="17" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A17" s="0" t="s">
-        <v>222</v>
+        <v>238</v>
       </c>
     </row>
     <row r="18" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A18" s="0" t="s">
-        <v>222</v>
+        <v>238</v>
       </c>
     </row>
     <row r="19" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A19" s="0" t="s">
-        <v>222</v>
+        <v>238</v>
       </c>
     </row>
     <row r="20" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A20" s="0" t="s">
-        <v>223</v>
+        <v>239</v>
       </c>
     </row>
     <row r="21" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A21" s="0" t="s">
-        <v>223</v>
+        <v>239</v>
       </c>
     </row>
   </sheetData>
@@ -1538,183 +1638,183 @@
   <sheetData>
     <row r="1" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A1" s="1" t="s">
-        <v>224</v>
+        <v>240</v>
       </c>
       <c r="B1" s="1"/>
     </row>
     <row r="2" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A2" s="0" t="s">
-        <v>216</v>
+        <v>232</v>
       </c>
     </row>
     <row r="3" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A3" s="0" t="s">
-        <v>216</v>
+        <v>232</v>
       </c>
     </row>
     <row r="4" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A4" s="0" t="s">
-        <v>225</v>
+        <v>241</v>
       </c>
     </row>
     <row r="5" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A5" s="0" t="s">
-        <v>225</v>
+        <v>241</v>
       </c>
     </row>
     <row r="6" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A6" s="0" t="s">
-        <v>226</v>
+        <v>242</v>
       </c>
     </row>
     <row r="7" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A7" s="0" t="s">
-        <v>226</v>
+        <v>242</v>
       </c>
     </row>
     <row r="8" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A8" s="0" t="s">
-        <v>226</v>
+        <v>242</v>
       </c>
     </row>
     <row r="9" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A9" s="0" t="s">
-        <v>226</v>
+        <v>242</v>
       </c>
     </row>
     <row r="10" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A10" s="0" t="s">
-        <v>226</v>
+        <v>242</v>
       </c>
     </row>
     <row r="11" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A11" s="0" t="s">
-        <v>226</v>
+        <v>242</v>
       </c>
     </row>
     <row r="12" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A12" s="0" t="s">
-        <v>219</v>
+        <v>235</v>
       </c>
     </row>
     <row r="13" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A13" s="0" t="s">
-        <v>219</v>
+        <v>235</v>
       </c>
     </row>
     <row r="14" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A14" s="0" t="s">
-        <v>219</v>
+        <v>235</v>
       </c>
     </row>
     <row r="15" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A15" s="0" t="s">
-        <v>227</v>
+        <v>243</v>
       </c>
     </row>
     <row r="16" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A16" s="0" t="s">
-        <v>228</v>
+        <v>244</v>
       </c>
     </row>
     <row r="17" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A17" s="0" t="s">
-        <v>228</v>
+        <v>244</v>
       </c>
     </row>
     <row r="18" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A18" s="0" t="s">
-        <v>228</v>
+        <v>244</v>
       </c>
     </row>
     <row r="19" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A19" s="0" t="s">
-        <v>228</v>
+        <v>244</v>
       </c>
     </row>
     <row r="20" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A20" s="0" t="s">
-        <v>228</v>
+        <v>244</v>
       </c>
     </row>
     <row r="21" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A21" s="0" t="s">
-        <v>228</v>
+        <v>244</v>
       </c>
     </row>
     <row r="22" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A22" s="0" t="s">
-        <v>221</v>
+        <v>237</v>
       </c>
     </row>
     <row r="23" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A23" s="0" t="s">
-        <v>221</v>
+        <v>237</v>
       </c>
     </row>
     <row r="24" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A24" s="0" t="s">
-        <v>221</v>
+        <v>237</v>
       </c>
     </row>
     <row r="25" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A25" s="0" t="s">
-        <v>221</v>
+        <v>237</v>
       </c>
     </row>
     <row r="26" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A26" s="0" t="s">
-        <v>221</v>
+        <v>237</v>
       </c>
     </row>
     <row r="27" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A27" s="0" t="s">
-        <v>221</v>
+        <v>237</v>
       </c>
     </row>
     <row r="28" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A28" s="0" t="s">
-        <v>229</v>
+        <v>245</v>
       </c>
     </row>
     <row r="29" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A29" s="0" t="s">
-        <v>222</v>
+        <v>238</v>
       </c>
     </row>
     <row r="30" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A30" s="0" t="s">
-        <v>230</v>
+        <v>246</v>
       </c>
     </row>
     <row r="31" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A31" s="0" t="s">
-        <v>230</v>
+        <v>246</v>
       </c>
     </row>
     <row r="32" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A32" s="0" t="s">
-        <v>230</v>
+        <v>246</v>
       </c>
     </row>
     <row r="33" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A33" s="0" t="s">
-        <v>230</v>
+        <v>246</v>
       </c>
     </row>
     <row r="34" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A34" s="0" t="s">
-        <v>230</v>
+        <v>246</v>
       </c>
     </row>
     <row r="35" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A35" s="0" t="s">
-        <v>230</v>
+        <v>246</v>
       </c>
     </row>
     <row r="36" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A36" s="0" t="s">
-        <v>230</v>
+        <v>246</v>
       </c>
     </row>
   </sheetData>
@@ -1751,39 +1851,39 @@
   <sheetData>
     <row r="1" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A1" s="1" t="s">
-        <v>231</v>
+        <v>247</v>
       </c>
       <c r="B1" s="1" t="s">
-        <v>35</v>
+        <v>2</v>
       </c>
       <c r="C1" s="1" t="s">
-        <v>232</v>
+        <v>248</v>
       </c>
       <c r="D1" s="1" t="s">
-        <v>233</v>
+        <v>249</v>
       </c>
       <c r="E1" s="1"/>
     </row>
     <row r="2" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A2" s="0" t="s">
-        <v>234</v>
+        <v>250</v>
       </c>
       <c r="B2" s="0" t="s">
-        <v>235</v>
+        <v>251</v>
       </c>
       <c r="C2" s="0" t="n">
         <v>15</v>
       </c>
       <c r="D2" s="0" t="s">
-        <v>236</v>
+        <v>252</v>
       </c>
     </row>
     <row r="3" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A3" s="0" t="s">
-        <v>237</v>
+        <v>253</v>
       </c>
       <c r="B3" s="0" t="s">
-        <v>238</v>
+        <v>254</v>
       </c>
       <c r="C3" s="0" t="n">
         <v>15</v>
@@ -1791,10 +1891,10 @@
     </row>
     <row r="4" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A4" s="0" t="s">
-        <v>239</v>
+        <v>255</v>
       </c>
       <c r="B4" s="0" t="s">
-        <v>240</v>
+        <v>256</v>
       </c>
       <c r="C4" s="0" t="n">
         <v>10</v>
@@ -1802,123 +1902,123 @@
     </row>
     <row r="5" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A5" s="0" t="s">
-        <v>241</v>
+        <v>257</v>
       </c>
       <c r="B5" s="0" t="s">
-        <v>242</v>
+        <v>258</v>
       </c>
       <c r="C5" s="0" t="n">
         <v>15</v>
       </c>
       <c r="D5" s="0" t="s">
-        <v>243</v>
+        <v>259</v>
       </c>
     </row>
     <row r="6" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A6" s="0" t="s">
-        <v>244</v>
+        <v>260</v>
       </c>
       <c r="B6" s="0" t="s">
-        <v>245</v>
+        <v>261</v>
       </c>
       <c r="C6" s="0" t="n">
         <v>15</v>
       </c>
       <c r="D6" s="0" t="s">
-        <v>246</v>
+        <v>262</v>
       </c>
     </row>
     <row r="7" customFormat="false" ht="30" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A7" s="0" t="s">
-        <v>247</v>
+        <v>263</v>
       </c>
       <c r="B7" s="5" t="s">
-        <v>248</v>
+        <v>264</v>
       </c>
       <c r="C7" s="0" t="n">
         <v>15</v>
       </c>
       <c r="D7" s="0" t="s">
-        <v>249</v>
+        <v>265</v>
       </c>
     </row>
     <row r="8" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A8" s="0" t="s">
-        <v>250</v>
+        <v>266</v>
       </c>
       <c r="B8" s="0" t="s">
-        <v>251</v>
+        <v>267</v>
       </c>
       <c r="C8" s="0" t="n">
         <v>15</v>
       </c>
       <c r="D8" s="0" t="s">
-        <v>252</v>
+        <v>268</v>
       </c>
     </row>
     <row r="9" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A9" s="0" t="s">
-        <v>253</v>
+        <v>269</v>
       </c>
       <c r="B9" s="0" t="s">
-        <v>254</v>
+        <v>270</v>
       </c>
       <c r="C9" s="0" t="n">
         <v>15</v>
       </c>
       <c r="D9" s="0" t="s">
-        <v>255</v>
+        <v>271</v>
       </c>
     </row>
     <row r="10" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A10" s="0" t="s">
-        <v>256</v>
+        <v>272</v>
       </c>
       <c r="B10" s="0" t="s">
-        <v>257</v>
+        <v>273</v>
       </c>
       <c r="C10" s="0" t="n">
         <v>15</v>
       </c>
       <c r="D10" s="0" t="s">
-        <v>258</v>
+        <v>274</v>
       </c>
     </row>
     <row r="12" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A12" s="1" t="s">
-        <v>259</v>
+        <v>275</v>
       </c>
       <c r="B12" s="1" t="s">
-        <v>35</v>
+        <v>2</v>
       </c>
       <c r="C12" s="1" t="s">
-        <v>232</v>
+        <v>248</v>
       </c>
       <c r="D12" s="1" t="s">
-        <v>233</v>
+        <v>249</v>
       </c>
       <c r="E12" s="1"/>
     </row>
     <row r="13" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A13" s="0" t="s">
-        <v>260</v>
+        <v>276</v>
       </c>
       <c r="B13" s="0" t="s">
-        <v>261</v>
+        <v>277</v>
       </c>
       <c r="C13" s="0" t="n">
         <v>20</v>
       </c>
       <c r="D13" s="0" t="s">
-        <v>262</v>
+        <v>278</v>
       </c>
     </row>
     <row r="14" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A14" s="0" t="s">
-        <v>263</v>
+        <v>279</v>
       </c>
       <c r="B14" s="0" t="s">
-        <v>264</v>
+        <v>280</v>
       </c>
       <c r="C14" s="0" t="n">
         <v>15</v>
@@ -1926,179 +2026,179 @@
     </row>
     <row r="15" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A15" s="0" t="s">
-        <v>265</v>
+        <v>281</v>
       </c>
       <c r="B15" s="0" t="s">
-        <v>266</v>
+        <v>282</v>
       </c>
       <c r="C15" s="0" t="n">
         <v>20</v>
       </c>
       <c r="D15" s="0" t="s">
-        <v>267</v>
+        <v>283</v>
       </c>
     </row>
     <row r="16" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A16" s="0" t="s">
-        <v>268</v>
+        <v>284</v>
       </c>
       <c r="B16" s="0" t="s">
-        <v>269</v>
+        <v>285</v>
       </c>
       <c r="C16" s="0" t="n">
         <v>20</v>
       </c>
       <c r="D16" s="0" t="s">
-        <v>270</v>
+        <v>286</v>
       </c>
     </row>
     <row r="17" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A17" s="0" t="s">
-        <v>271</v>
+        <v>287</v>
       </c>
       <c r="B17" s="0" t="s">
-        <v>272</v>
+        <v>288</v>
       </c>
       <c r="C17" s="0" t="n">
         <v>20</v>
       </c>
       <c r="D17" s="0" t="s">
-        <v>273</v>
+        <v>289</v>
       </c>
     </row>
     <row r="18" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A18" s="0" t="s">
-        <v>274</v>
+        <v>290</v>
       </c>
       <c r="B18" s="0" t="s">
-        <v>275</v>
+        <v>291</v>
       </c>
       <c r="C18" s="0" t="n">
         <v>20</v>
       </c>
       <c r="D18" s="0" t="s">
-        <v>276</v>
+        <v>292</v>
       </c>
     </row>
     <row r="19" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A19" s="0" t="s">
-        <v>277</v>
+        <v>293</v>
       </c>
       <c r="B19" s="0" t="s">
-        <v>278</v>
+        <v>294</v>
       </c>
       <c r="C19" s="0" t="n">
         <v>20</v>
       </c>
       <c r="D19" s="0" t="s">
-        <v>279</v>
+        <v>295</v>
       </c>
     </row>
     <row r="20" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A20" s="0" t="s">
-        <v>280</v>
+        <v>296</v>
       </c>
       <c r="B20" s="0" t="s">
-        <v>281</v>
+        <v>297</v>
       </c>
       <c r="C20" s="0" t="n">
         <v>20</v>
       </c>
       <c r="D20" s="0" t="s">
-        <v>282</v>
+        <v>298</v>
       </c>
     </row>
     <row r="21" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A21" s="0" t="s">
-        <v>283</v>
+        <v>299</v>
       </c>
       <c r="B21" s="0" t="s">
-        <v>284</v>
+        <v>300</v>
       </c>
       <c r="C21" s="0" t="n">
         <v>20</v>
       </c>
       <c r="D21" s="0" t="s">
-        <v>285</v>
+        <v>301</v>
       </c>
     </row>
     <row r="23" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A23" s="1" t="s">
-        <v>286</v>
+        <v>302</v>
       </c>
       <c r="B23" s="1" t="s">
-        <v>35</v>
+        <v>2</v>
       </c>
       <c r="C23" s="1" t="s">
-        <v>232</v>
+        <v>248</v>
       </c>
       <c r="D23" s="1" t="s">
-        <v>233</v>
+        <v>249</v>
       </c>
       <c r="E23" s="1"/>
     </row>
     <row r="24" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A24" s="0" t="s">
-        <v>287</v>
+        <v>303</v>
       </c>
       <c r="B24" s="0" t="s">
-        <v>288</v>
+        <v>304</v>
       </c>
       <c r="C24" s="0" t="n">
         <v>25</v>
       </c>
       <c r="D24" s="0" t="s">
-        <v>289</v>
+        <v>305</v>
       </c>
     </row>
     <row r="25" customFormat="false" ht="30" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A25" s="0" t="s">
-        <v>290</v>
+        <v>306</v>
       </c>
       <c r="B25" s="5" t="s">
-        <v>291</v>
+        <v>307</v>
       </c>
       <c r="C25" s="0" t="n">
         <v>25</v>
       </c>
       <c r="D25" s="0" t="s">
-        <v>292</v>
+        <v>308</v>
       </c>
     </row>
     <row r="26" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A26" s="0" t="s">
-        <v>293</v>
+        <v>309</v>
       </c>
       <c r="B26" s="0" t="s">
-        <v>294</v>
+        <v>310</v>
       </c>
       <c r="C26" s="0" t="n">
         <v>25</v>
       </c>
       <c r="D26" s="0" t="s">
-        <v>295</v>
+        <v>311</v>
       </c>
     </row>
     <row r="27" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A27" s="0" t="s">
-        <v>296</v>
+        <v>312</v>
       </c>
       <c r="B27" s="0" t="s">
-        <v>297</v>
+        <v>313</v>
       </c>
       <c r="C27" s="0" t="n">
         <v>25</v>
       </c>
       <c r="D27" s="0" t="s">
-        <v>298</v>
+        <v>314</v>
       </c>
     </row>
     <row r="28" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A28" s="0" t="s">
-        <v>299</v>
+        <v>315</v>
       </c>
       <c r="B28" s="0" t="s">
-        <v>300</v>
+        <v>316</v>
       </c>
       <c r="C28" s="0" t="n">
         <v>25</v>
@@ -2106,52 +2206,52 @@
     </row>
     <row r="29" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A29" s="0" t="s">
-        <v>301</v>
+        <v>317</v>
       </c>
       <c r="B29" s="0" t="s">
-        <v>302</v>
+        <v>318</v>
       </c>
       <c r="C29" s="0" t="n">
         <v>25</v>
       </c>
       <c r="D29" s="0" t="s">
-        <v>303</v>
+        <v>319</v>
       </c>
     </row>
     <row r="30" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A30" s="0" t="s">
-        <v>304</v>
+        <v>320</v>
       </c>
       <c r="B30" s="0" t="s">
-        <v>305</v>
+        <v>321</v>
       </c>
       <c r="C30" s="0" t="n">
         <v>25</v>
       </c>
       <c r="D30" s="0" t="s">
-        <v>306</v>
+        <v>322</v>
       </c>
     </row>
     <row r="31" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A31" s="0" t="s">
-        <v>307</v>
+        <v>323</v>
       </c>
       <c r="B31" s="0" t="s">
-        <v>308</v>
+        <v>324</v>
       </c>
       <c r="C31" s="0" t="n">
         <v>25</v>
       </c>
       <c r="D31" s="0" t="s">
-        <v>309</v>
+        <v>325</v>
       </c>
     </row>
     <row r="32" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A32" s="0" t="s">
-        <v>310</v>
+        <v>326</v>
       </c>
       <c r="B32" s="0" t="s">
-        <v>311</v>
+        <v>327</v>
       </c>
       <c r="C32" s="0" t="n">
         <v>20</v>
@@ -2187,7 +2287,7 @@
   <sheetData>
     <row r="1" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A1" s="1" t="s">
-        <v>111</v>
+        <v>127</v>
       </c>
       <c r="B1" s="1"/>
     </row>
@@ -2358,50 +2458,50 @@
   <sheetData>
     <row r="1" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A1" s="1" t="s">
-        <v>312</v>
+        <v>328</v>
       </c>
       <c r="B1" s="1" t="s">
-        <v>35</v>
+        <v>2</v>
       </c>
     </row>
     <row r="2" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A2" s="0" t="s">
-        <v>313</v>
+        <v>329</v>
       </c>
       <c r="B2" s="0" t="s">
-        <v>314</v>
+        <v>330</v>
       </c>
     </row>
     <row r="3" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A3" s="0" t="s">
-        <v>315</v>
+        <v>331</v>
       </c>
       <c r="B3" s="0" t="s">
-        <v>316</v>
+        <v>332</v>
       </c>
     </row>
     <row r="4" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A4" s="0" t="s">
-        <v>317</v>
+        <v>333</v>
       </c>
       <c r="B4" s="0" t="s">
-        <v>318</v>
+        <v>334</v>
       </c>
     </row>
     <row r="5" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A5" s="0" t="s">
-        <v>319</v>
+        <v>335</v>
       </c>
       <c r="B5" s="0" t="s">
-        <v>320</v>
+        <v>336</v>
       </c>
     </row>
     <row r="6" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A6" s="0" t="s">
-        <v>321</v>
+        <v>337</v>
       </c>
       <c r="B6" s="0" t="s">
-        <v>322</v>
+        <v>338</v>
       </c>
     </row>
     <row r="16" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
@@ -2439,70 +2539,70 @@
   <sheetData>
     <row r="1" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A1" s="1" t="s">
-        <v>323</v>
+        <v>339</v>
       </c>
       <c r="B1" s="1" t="s">
-        <v>35</v>
+        <v>2</v>
       </c>
     </row>
     <row r="2" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A2" s="0" t="s">
-        <v>33</v>
+        <v>49</v>
       </c>
     </row>
     <row r="3" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A3" s="0" t="s">
-        <v>21</v>
+        <v>31</v>
       </c>
     </row>
     <row r="4" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A4" s="0" t="s">
-        <v>27</v>
+        <v>40</v>
       </c>
     </row>
     <row r="5" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A5" s="0" t="s">
-        <v>3</v>
+        <v>4</v>
       </c>
     </row>
     <row r="6" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A6" s="0" t="s">
-        <v>25</v>
+        <v>37</v>
       </c>
     </row>
     <row r="7" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A7" s="0" t="s">
-        <v>324</v>
+        <v>340</v>
       </c>
     </row>
     <row r="8" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A8" s="0" t="s">
-        <v>17</v>
+        <v>25</v>
       </c>
     </row>
     <row r="9" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A9" s="0" t="s">
-        <v>31</v>
+        <v>46</v>
       </c>
     </row>
     <row r="10" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A10" s="0" t="s">
-        <v>325</v>
+        <v>341</v>
       </c>
     </row>
     <row r="11" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A11" s="0" t="s">
-        <v>15</v>
+        <v>22</v>
       </c>
     </row>
     <row r="12" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A12" s="0" t="s">
-        <v>9</v>
+        <v>13</v>
       </c>
     </row>
     <row r="13" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A13" s="0" t="s">
-        <v>13</v>
+        <v>19</v>
       </c>
     </row>
   </sheetData>
@@ -2535,75 +2635,75 @@
   <sheetData>
     <row r="1" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A1" s="1" t="s">
-        <v>323</v>
+        <v>339</v>
       </c>
       <c r="B1" s="1" t="s">
-        <v>35</v>
+        <v>2</v>
       </c>
     </row>
     <row r="2" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A2" s="0" t="s">
-        <v>326</v>
+        <v>342</v>
       </c>
     </row>
     <row r="3" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A3" s="0" t="s">
-        <v>23</v>
+        <v>34</v>
       </c>
     </row>
     <row r="4" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A4" s="0" t="s">
-        <v>11</v>
+        <v>16</v>
       </c>
     </row>
     <row r="5" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A5" s="0" t="s">
-        <v>19</v>
+        <v>28</v>
       </c>
     </row>
     <row r="6" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A6" s="0" t="s">
-        <v>327</v>
+        <v>343</v>
       </c>
     </row>
     <row r="7" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A7" s="0" t="s">
-        <v>7</v>
+        <v>10</v>
       </c>
     </row>
     <row r="8" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A8" s="0" t="s">
-        <v>5</v>
+        <v>7</v>
       </c>
     </row>
     <row r="9" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A9" s="0" t="s">
-        <v>328</v>
+        <v>344</v>
       </c>
     </row>
     <row r="10" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A10" s="0" t="s">
-        <v>329</v>
+        <v>345</v>
       </c>
     </row>
     <row r="11" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A11" s="0" t="s">
-        <v>330</v>
+        <v>346</v>
       </c>
     </row>
     <row r="12" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A12" s="0" t="s">
-        <v>331</v>
+        <v>347</v>
       </c>
     </row>
     <row r="13" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A13" s="0" t="s">
-        <v>332</v>
+        <v>348</v>
       </c>
     </row>
     <row r="14" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A14" s="0" t="s">
-        <v>333</v>
+        <v>349</v>
       </c>
     </row>
   </sheetData>
@@ -2636,65 +2736,65 @@
   <sheetData>
     <row r="1" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A1" s="1" t="s">
-        <v>323</v>
+        <v>339</v>
       </c>
       <c r="B1" s="1" t="s">
-        <v>35</v>
+        <v>2</v>
       </c>
     </row>
     <row r="2" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A2" s="0" t="s">
-        <v>334</v>
+        <v>350</v>
       </c>
     </row>
     <row r="3" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A3" s="0" t="s">
-        <v>335</v>
+        <v>351</v>
       </c>
     </row>
     <row r="4" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A4" s="0" t="s">
-        <v>29</v>
+        <v>43</v>
       </c>
     </row>
     <row r="5" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A5" s="0" t="s">
-        <v>336</v>
+        <v>352</v>
       </c>
     </row>
     <row r="6" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A6" s="0" t="s">
-        <v>337</v>
+        <v>353</v>
       </c>
     </row>
     <row r="7" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A7" s="0" t="s">
-        <v>338</v>
+        <v>354</v>
       </c>
     </row>
     <row r="8" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A8" s="0" t="s">
-        <v>339</v>
+        <v>355</v>
       </c>
     </row>
     <row r="9" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A9" s="0" t="s">
-        <v>340</v>
+        <v>356</v>
       </c>
     </row>
     <row r="10" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A10" s="0" t="s">
-        <v>341</v>
+        <v>357</v>
       </c>
     </row>
     <row r="11" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A11" s="0" t="s">
-        <v>342</v>
+        <v>358</v>
       </c>
     </row>
     <row r="12" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A12" s="0" t="s">
-        <v>343</v>
+        <v>359</v>
       </c>
     </row>
   </sheetData>
@@ -2727,55 +2827,55 @@
   <sheetData>
     <row r="1" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A1" s="1" t="s">
-        <v>323</v>
+        <v>339</v>
       </c>
       <c r="B1" s="1" t="s">
-        <v>35</v>
+        <v>2</v>
       </c>
     </row>
     <row r="2" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A2" s="0" t="s">
-        <v>344</v>
+        <v>360</v>
       </c>
     </row>
     <row r="3" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A3" s="0" t="s">
-        <v>345</v>
+        <v>361</v>
       </c>
     </row>
     <row r="4" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A4" s="0" t="s">
-        <v>346</v>
+        <v>362</v>
       </c>
     </row>
     <row r="5" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A5" s="0" t="s">
-        <v>347</v>
+        <v>363</v>
       </c>
     </row>
     <row r="6" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A6" s="0" t="s">
-        <v>348</v>
+        <v>364</v>
       </c>
     </row>
     <row r="7" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A7" s="0" t="s">
-        <v>349</v>
+        <v>365</v>
       </c>
     </row>
     <row r="8" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A8" s="0" t="s">
-        <v>350</v>
+        <v>366</v>
       </c>
     </row>
     <row r="9" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A9" s="0" t="s">
-        <v>351</v>
+        <v>367</v>
       </c>
     </row>
     <row r="10" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A10" s="0" t="s">
-        <v>350</v>
+        <v>366</v>
       </c>
     </row>
   </sheetData>
@@ -2809,253 +2909,253 @@
   <sheetData>
     <row r="1" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A1" s="1" t="s">
-        <v>34</v>
+        <v>51</v>
       </c>
       <c r="B1" s="1" t="s">
-        <v>35</v>
+        <v>2</v>
       </c>
       <c r="C1" s="1"/>
     </row>
     <row r="2" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A2" s="2" t="s">
-        <v>36</v>
+        <v>52</v>
       </c>
       <c r="B2" s="2" t="s">
-        <v>37</v>
+        <v>53</v>
       </c>
       <c r="C2" s="2"/>
     </row>
     <row r="3" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A3" s="2" t="s">
-        <v>36</v>
+        <v>52</v>
       </c>
       <c r="B3" s="2" t="s">
-        <v>37</v>
+        <v>53</v>
       </c>
       <c r="C3" s="2"/>
     </row>
     <row r="4" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A4" s="2" t="s">
-        <v>36</v>
+        <v>52</v>
       </c>
       <c r="B4" s="2" t="s">
-        <v>37</v>
+        <v>53</v>
       </c>
       <c r="C4" s="2"/>
     </row>
     <row r="5" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A5" s="2" t="s">
-        <v>38</v>
+        <v>54</v>
       </c>
       <c r="B5" s="2" t="s">
-        <v>39</v>
+        <v>55</v>
       </c>
       <c r="C5" s="2"/>
     </row>
     <row r="6" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A6" s="2" t="s">
-        <v>38</v>
+        <v>54</v>
       </c>
       <c r="B6" s="2" t="s">
-        <v>39</v>
+        <v>55</v>
       </c>
       <c r="C6" s="2"/>
     </row>
     <row r="7" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A7" s="2" t="s">
-        <v>40</v>
+        <v>56</v>
       </c>
       <c r="B7" s="2" t="s">
-        <v>41</v>
+        <v>57</v>
       </c>
       <c r="C7" s="2"/>
     </row>
     <row r="8" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A8" s="2" t="s">
-        <v>40</v>
+        <v>56</v>
       </c>
       <c r="B8" s="2" t="s">
-        <v>41</v>
+        <v>57</v>
       </c>
       <c r="C8" s="2"/>
     </row>
     <row r="9" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A9" s="2" t="s">
-        <v>42</v>
+        <v>58</v>
       </c>
       <c r="B9" s="2" t="s">
-        <v>43</v>
+        <v>59</v>
       </c>
       <c r="C9" s="2"/>
     </row>
     <row r="10" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A10" s="2" t="s">
-        <v>42</v>
+        <v>58</v>
       </c>
       <c r="B10" s="2" t="s">
-        <v>43</v>
+        <v>59</v>
       </c>
       <c r="C10" s="2"/>
     </row>
     <row r="11" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A11" s="2" t="s">
-        <v>44</v>
+        <v>60</v>
       </c>
       <c r="B11" s="2" t="s">
-        <v>45</v>
+        <v>61</v>
       </c>
       <c r="C11" s="2"/>
     </row>
     <row r="12" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A12" s="2" t="s">
-        <v>44</v>
+        <v>60</v>
       </c>
       <c r="B12" s="2" t="s">
-        <v>45</v>
+        <v>61</v>
       </c>
       <c r="C12" s="2"/>
     </row>
     <row r="13" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A13" s="2" t="s">
-        <v>46</v>
+        <v>62</v>
       </c>
       <c r="B13" s="2" t="s">
-        <v>47</v>
+        <v>63</v>
       </c>
       <c r="C13" s="2"/>
     </row>
     <row r="14" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A14" s="2" t="s">
-        <v>48</v>
+        <v>64</v>
       </c>
       <c r="B14" s="2" t="s">
-        <v>49</v>
+        <v>65</v>
       </c>
       <c r="C14" s="2"/>
     </row>
     <row r="15" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A15" s="2" t="s">
-        <v>48</v>
+        <v>64</v>
       </c>
       <c r="B15" s="2" t="s">
-        <v>49</v>
+        <v>65</v>
       </c>
       <c r="C15" s="2"/>
     </row>
     <row r="16" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A16" s="2" t="s">
-        <v>50</v>
+        <v>66</v>
       </c>
       <c r="B16" s="2" t="s">
-        <v>51</v>
+        <v>67</v>
       </c>
       <c r="C16" s="2"/>
     </row>
     <row r="17" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A17" s="2" t="s">
-        <v>50</v>
+        <v>66</v>
       </c>
       <c r="B17" s="2" t="s">
-        <v>51</v>
+        <v>67</v>
       </c>
       <c r="C17" s="2"/>
     </row>
     <row r="18" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A18" s="2" t="s">
-        <v>52</v>
+        <v>68</v>
       </c>
       <c r="B18" s="2" t="s">
-        <v>53</v>
+        <v>69</v>
       </c>
       <c r="C18" s="2"/>
     </row>
     <row r="19" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A19" s="2" t="s">
-        <v>52</v>
+        <v>68</v>
       </c>
       <c r="B19" s="2" t="s">
-        <v>53</v>
+        <v>69</v>
       </c>
       <c r="C19" s="2"/>
     </row>
     <row r="20" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A20" s="2" t="s">
-        <v>52</v>
+        <v>68</v>
       </c>
       <c r="B20" s="2" t="s">
-        <v>53</v>
+        <v>69</v>
       </c>
       <c r="C20" s="2"/>
     </row>
     <row r="21" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A21" s="2" t="s">
-        <v>54</v>
+        <v>70</v>
       </c>
       <c r="B21" s="2" t="s">
-        <v>55</v>
+        <v>71</v>
       </c>
       <c r="C21" s="2"/>
     </row>
     <row r="22" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A22" s="2" t="s">
-        <v>54</v>
+        <v>70</v>
       </c>
       <c r="B22" s="2" t="s">
-        <v>55</v>
+        <v>71</v>
       </c>
       <c r="C22" s="2"/>
     </row>
     <row r="23" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A23" s="2" t="s">
-        <v>56</v>
+        <v>72</v>
       </c>
       <c r="B23" s="2" t="s">
-        <v>57</v>
+        <v>73</v>
       </c>
       <c r="C23" s="2"/>
     </row>
     <row r="24" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A24" s="2" t="s">
-        <v>56</v>
+        <v>72</v>
       </c>
       <c r="B24" s="2" t="s">
-        <v>57</v>
+        <v>73</v>
       </c>
       <c r="C24" s="2"/>
     </row>
     <row r="25" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A25" s="2" t="s">
-        <v>58</v>
+        <v>74</v>
       </c>
       <c r="B25" s="2" t="s">
-        <v>59</v>
+        <v>75</v>
       </c>
       <c r="C25" s="2"/>
     </row>
     <row r="26" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A26" s="2" t="s">
-        <v>60</v>
+        <v>76</v>
       </c>
       <c r="B26" s="2" t="s">
-        <v>61</v>
+        <v>77</v>
       </c>
       <c r="C26" s="2"/>
     </row>
     <row r="27" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A27" s="2" t="s">
-        <v>60</v>
+        <v>76</v>
       </c>
       <c r="B27" s="2" t="s">
-        <v>61</v>
+        <v>77</v>
       </c>
       <c r="C27" s="2"/>
     </row>
     <row r="28" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A28" s="2" t="s">
-        <v>60</v>
+        <v>76</v>
       </c>
       <c r="B28" s="2" t="s">
-        <v>61</v>
+        <v>77</v>
       </c>
       <c r="C28" s="2"/>
     </row>
@@ -3090,235 +3190,235 @@
   <sheetData>
     <row r="1" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A1" s="1" t="s">
-        <v>34</v>
+        <v>51</v>
       </c>
       <c r="B1" s="1" t="s">
-        <v>35</v>
+        <v>2</v>
       </c>
       <c r="C1" s="1"/>
     </row>
     <row r="2" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A2" s="2" t="s">
-        <v>62</v>
+        <v>78</v>
       </c>
       <c r="B2" s="2" t="s">
-        <v>63</v>
+        <v>79</v>
       </c>
       <c r="C2" s="2"/>
     </row>
     <row r="3" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A3" s="2" t="s">
-        <v>62</v>
+        <v>78</v>
       </c>
       <c r="B3" s="2" t="s">
-        <v>63</v>
+        <v>79</v>
       </c>
       <c r="C3" s="2"/>
     </row>
     <row r="4" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A4" s="2" t="s">
-        <v>62</v>
+        <v>78</v>
       </c>
       <c r="B4" s="2" t="s">
-        <v>63</v>
+        <v>79</v>
       </c>
       <c r="C4" s="2"/>
     </row>
     <row r="5" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A5" s="2" t="s">
-        <v>64</v>
+        <v>80</v>
       </c>
       <c r="B5" s="2" t="s">
-        <v>65</v>
+        <v>81</v>
       </c>
       <c r="C5" s="2"/>
     </row>
     <row r="6" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A6" s="2" t="s">
-        <v>66</v>
+        <v>82</v>
       </c>
       <c r="B6" s="2" t="s">
-        <v>67</v>
+        <v>83</v>
       </c>
       <c r="C6" s="2"/>
     </row>
     <row r="7" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A7" s="2" t="s">
-        <v>66</v>
+        <v>82</v>
       </c>
       <c r="B7" s="2" t="s">
-        <v>67</v>
+        <v>83</v>
       </c>
       <c r="C7" s="2"/>
     </row>
     <row r="8" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A8" s="2" t="s">
-        <v>68</v>
+        <v>84</v>
       </c>
       <c r="B8" s="2" t="s">
-        <v>69</v>
+        <v>85</v>
       </c>
       <c r="C8" s="2"/>
     </row>
     <row r="9" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A9" s="2" t="s">
-        <v>68</v>
+        <v>84</v>
       </c>
       <c r="B9" s="2" t="s">
-        <v>69</v>
+        <v>85</v>
       </c>
       <c r="C9" s="2"/>
     </row>
     <row r="10" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A10" s="2" t="s">
-        <v>70</v>
+        <v>86</v>
       </c>
       <c r="B10" s="2" t="s">
-        <v>71</v>
+        <v>87</v>
       </c>
       <c r="C10" s="2"/>
     </row>
     <row r="11" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A11" s="2" t="s">
-        <v>72</v>
+        <v>88</v>
       </c>
       <c r="B11" s="2" t="s">
-        <v>73</v>
+        <v>89</v>
       </c>
       <c r="C11" s="2"/>
     </row>
     <row r="12" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A12" s="2" t="s">
-        <v>74</v>
+        <v>90</v>
       </c>
       <c r="B12" s="2" t="s">
-        <v>75</v>
+        <v>91</v>
       </c>
       <c r="C12" s="2"/>
     </row>
     <row r="13" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A13" s="2" t="s">
-        <v>74</v>
+        <v>90</v>
       </c>
       <c r="B13" s="2" t="s">
-        <v>75</v>
+        <v>91</v>
       </c>
       <c r="C13" s="2"/>
     </row>
     <row r="14" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A14" s="2" t="s">
-        <v>76</v>
+        <v>92</v>
       </c>
       <c r="B14" s="2" t="s">
-        <v>77</v>
+        <v>93</v>
       </c>
       <c r="C14" s="2"/>
     </row>
     <row r="15" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A15" s="2" t="s">
-        <v>76</v>
+        <v>92</v>
       </c>
       <c r="B15" s="2" t="s">
-        <v>77</v>
+        <v>93</v>
       </c>
       <c r="C15" s="2"/>
     </row>
     <row r="16" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A16" s="2" t="s">
-        <v>76</v>
+        <v>92</v>
       </c>
       <c r="B16" s="2" t="s">
-        <v>77</v>
+        <v>93</v>
       </c>
       <c r="C16" s="2"/>
     </row>
     <row r="17" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A17" s="2" t="s">
-        <v>78</v>
+        <v>94</v>
       </c>
       <c r="B17" s="2" t="s">
-        <v>79</v>
+        <v>95</v>
       </c>
       <c r="C17" s="2"/>
     </row>
     <row r="18" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A18" s="2" t="s">
-        <v>80</v>
+        <v>96</v>
       </c>
       <c r="B18" s="2" t="s">
-        <v>81</v>
+        <v>97</v>
       </c>
       <c r="C18" s="2"/>
     </row>
     <row r="19" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A19" s="2" t="s">
-        <v>80</v>
+        <v>96</v>
       </c>
       <c r="B19" s="2" t="s">
-        <v>81</v>
+        <v>97</v>
       </c>
       <c r="C19" s="2"/>
     </row>
     <row r="20" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A20" s="2" t="s">
-        <v>82</v>
+        <v>98</v>
       </c>
       <c r="B20" s="2" t="s">
-        <v>83</v>
+        <v>99</v>
       </c>
       <c r="C20" s="2"/>
     </row>
     <row r="21" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A21" s="2" t="s">
-        <v>82</v>
+        <v>98</v>
       </c>
       <c r="B21" s="2" t="s">
-        <v>83</v>
+        <v>99</v>
       </c>
       <c r="C21" s="2"/>
     </row>
     <row r="22" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A22" s="2" t="s">
-        <v>84</v>
+        <v>100</v>
       </c>
       <c r="B22" s="2" t="s">
-        <v>85</v>
+        <v>101</v>
       </c>
       <c r="C22" s="2"/>
     </row>
     <row r="23" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A23" s="2" t="s">
-        <v>84</v>
+        <v>100</v>
       </c>
       <c r="B23" s="2" t="s">
-        <v>85</v>
+        <v>101</v>
       </c>
       <c r="C23" s="2"/>
     </row>
     <row r="24" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A24" s="2" t="s">
-        <v>58</v>
+        <v>74</v>
       </c>
       <c r="B24" s="2" t="s">
-        <v>59</v>
+        <v>75</v>
       </c>
       <c r="C24" s="2"/>
     </row>
     <row r="25" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A25" s="2" t="s">
-        <v>86</v>
+        <v>102</v>
       </c>
       <c r="B25" s="2" t="s">
-        <v>87</v>
+        <v>103</v>
       </c>
       <c r="C25" s="2"/>
     </row>
     <row r="26" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A26" s="2" t="s">
-        <v>86</v>
+        <v>102</v>
       </c>
       <c r="B26" s="2" t="s">
-        <v>87</v>
+        <v>103</v>
       </c>
       <c r="C26" s="2"/>
     </row>
@@ -3353,163 +3453,163 @@
   <sheetData>
     <row r="1" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A1" s="1" t="s">
-        <v>34</v>
+        <v>51</v>
       </c>
       <c r="B1" s="1" t="s">
-        <v>35</v>
+        <v>2</v>
       </c>
       <c r="C1" s="1"/>
     </row>
     <row r="2" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A2" s="2" t="s">
-        <v>88</v>
+        <v>104</v>
       </c>
       <c r="B2" s="2" t="s">
-        <v>89</v>
+        <v>105</v>
       </c>
       <c r="C2" s="2"/>
     </row>
     <row r="3" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A3" s="2" t="s">
-        <v>88</v>
+        <v>104</v>
       </c>
       <c r="B3" s="2" t="s">
-        <v>89</v>
+        <v>105</v>
       </c>
       <c r="C3" s="2"/>
     </row>
     <row r="4" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A4" s="2" t="s">
-        <v>90</v>
+        <v>106</v>
       </c>
       <c r="B4" s="2" t="s">
-        <v>91</v>
+        <v>107</v>
       </c>
       <c r="C4" s="2"/>
     </row>
     <row r="5" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A5" s="2" t="s">
-        <v>92</v>
+        <v>108</v>
       </c>
       <c r="B5" s="2" t="s">
-        <v>93</v>
+        <v>109</v>
       </c>
       <c r="C5" s="2"/>
     </row>
     <row r="6" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A6" s="2" t="s">
-        <v>94</v>
+        <v>110</v>
       </c>
       <c r="B6" s="2" t="s">
-        <v>95</v>
+        <v>111</v>
       </c>
       <c r="C6" s="2"/>
     </row>
     <row r="7" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A7" s="2" t="s">
-        <v>94</v>
+        <v>110</v>
       </c>
       <c r="B7" s="2" t="s">
-        <v>95</v>
+        <v>111</v>
       </c>
       <c r="C7" s="2"/>
     </row>
     <row r="8" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A8" s="2" t="s">
-        <v>96</v>
+        <v>112</v>
       </c>
       <c r="B8" s="2" t="s">
-        <v>97</v>
+        <v>113</v>
       </c>
       <c r="C8" s="2"/>
     </row>
     <row r="9" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A9" s="2" t="s">
-        <v>98</v>
+        <v>114</v>
       </c>
       <c r="B9" s="2" t="s">
-        <v>99</v>
+        <v>115</v>
       </c>
       <c r="C9" s="2"/>
     </row>
     <row r="10" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A10" s="2" t="s">
-        <v>100</v>
+        <v>116</v>
       </c>
       <c r="B10" s="2" t="s">
-        <v>101</v>
+        <v>117</v>
       </c>
       <c r="C10" s="2"/>
     </row>
     <row r="11" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A11" s="2" t="s">
-        <v>100</v>
+        <v>116</v>
       </c>
       <c r="B11" s="2" t="s">
-        <v>101</v>
+        <v>117</v>
       </c>
       <c r="C11" s="2"/>
     </row>
     <row r="12" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A12" s="2" t="s">
-        <v>102</v>
+        <v>118</v>
       </c>
       <c r="B12" s="2" t="s">
-        <v>103</v>
+        <v>119</v>
       </c>
       <c r="C12" s="2"/>
     </row>
     <row r="13" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A13" s="2" t="s">
-        <v>102</v>
+        <v>118</v>
       </c>
       <c r="B13" s="2" t="s">
-        <v>103</v>
+        <v>119</v>
       </c>
       <c r="C13" s="2"/>
     </row>
     <row r="14" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A14" s="2" t="s">
-        <v>104</v>
+        <v>120</v>
       </c>
       <c r="B14" s="2" t="s">
-        <v>105</v>
+        <v>121</v>
       </c>
       <c r="C14" s="2"/>
     </row>
     <row r="15" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A15" s="2" t="s">
-        <v>104</v>
+        <v>120</v>
       </c>
       <c r="B15" s="2" t="s">
-        <v>105</v>
+        <v>121</v>
       </c>
       <c r="C15" s="2"/>
     </row>
     <row r="16" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A16" s="2" t="s">
-        <v>106</v>
+        <v>122</v>
       </c>
       <c r="B16" s="2" t="s">
-        <v>107</v>
+        <v>123</v>
       </c>
       <c r="C16" s="2"/>
     </row>
     <row r="17" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A17" s="2" t="s">
-        <v>108</v>
+        <v>124</v>
       </c>
       <c r="B17" s="2" t="s">
-        <v>109</v>
+        <v>125</v>
       </c>
       <c r="C17" s="2"/>
     </row>
     <row r="18" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A18" s="2" t="s">
-        <v>108</v>
+        <v>124</v>
       </c>
       <c r="B18" s="2" t="s">
-        <v>109</v>
+        <v>125</v>
       </c>
       <c r="C18" s="2"/>
     </row>
@@ -3531,7 +3631,7 @@
   </sheetPr>
   <dimension ref="A1:D43"/>
   <sheetViews>
-    <sheetView windowProtection="false" showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
+    <sheetView windowProtection="false" showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
       <selection pane="topLeft" activeCell="C22" activeCellId="0" sqref="C22"/>
     </sheetView>
   </sheetViews>
@@ -3546,517 +3646,517 @@
   <sheetData>
     <row r="1" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A1" s="3" t="s">
-        <v>110</v>
+        <v>126</v>
       </c>
       <c r="B1" s="3" t="s">
-        <v>111</v>
+        <v>127</v>
       </c>
       <c r="C1" s="3" t="s">
-        <v>35</v>
+        <v>2</v>
       </c>
       <c r="D1" s="3"/>
     </row>
     <row r="2" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A2" s="4" t="s">
-        <v>112</v>
+        <v>128</v>
       </c>
       <c r="B2" s="4" t="s">
-        <v>113</v>
+        <v>129</v>
       </c>
       <c r="C2" s="4" t="s">
-        <v>114</v>
+        <v>130</v>
       </c>
       <c r="D2" s="4"/>
     </row>
     <row r="3" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A3" s="4" t="s">
-        <v>115</v>
+        <v>131</v>
       </c>
       <c r="B3" s="4" t="s">
-        <v>113</v>
+        <v>129</v>
       </c>
       <c r="C3" s="4" t="s">
-        <v>116</v>
+        <v>132</v>
       </c>
       <c r="D3" s="4"/>
     </row>
     <row r="4" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A4" s="4" t="s">
-        <v>117</v>
+        <v>133</v>
       </c>
       <c r="B4" s="4" t="s">
-        <v>113</v>
+        <v>129</v>
       </c>
       <c r="C4" s="4" t="s">
-        <v>118</v>
+        <v>134</v>
       </c>
       <c r="D4" s="4"/>
     </row>
     <row r="5" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A5" s="4" t="s">
-        <v>119</v>
+        <v>135</v>
       </c>
       <c r="B5" s="4" t="s">
-        <v>113</v>
+        <v>129</v>
       </c>
       <c r="C5" s="4" t="s">
-        <v>120</v>
+        <v>136</v>
       </c>
       <c r="D5" s="4"/>
     </row>
     <row r="6" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A6" s="4" t="s">
-        <v>121</v>
+        <v>137</v>
       </c>
       <c r="B6" s="4" t="s">
-        <v>113</v>
+        <v>129</v>
       </c>
       <c r="C6" s="4" t="s">
-        <v>122</v>
+        <v>138</v>
       </c>
       <c r="D6" s="4"/>
     </row>
     <row r="7" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A7" s="4" t="s">
-        <v>123</v>
+        <v>139</v>
       </c>
       <c r="B7" s="4" t="s">
-        <v>113</v>
+        <v>129</v>
       </c>
       <c r="C7" s="4" t="s">
-        <v>124</v>
+        <v>140</v>
       </c>
       <c r="D7" s="4"/>
     </row>
     <row r="8" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A8" s="4" t="s">
-        <v>125</v>
+        <v>141</v>
       </c>
       <c r="B8" s="4" t="s">
-        <v>113</v>
+        <v>129</v>
       </c>
       <c r="C8" s="4" t="s">
-        <v>126</v>
+        <v>142</v>
       </c>
       <c r="D8" s="4"/>
     </row>
     <row r="9" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A9" s="4" t="s">
-        <v>127</v>
+        <v>143</v>
       </c>
       <c r="B9" s="4" t="s">
-        <v>128</v>
+        <v>144</v>
       </c>
       <c r="C9" s="4" t="s">
-        <v>129</v>
+        <v>145</v>
       </c>
       <c r="D9" s="4"/>
     </row>
     <row r="10" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A10" s="4" t="s">
-        <v>130</v>
+        <v>146</v>
       </c>
       <c r="B10" s="4" t="s">
-        <v>128</v>
+        <v>144</v>
       </c>
       <c r="C10" s="4" t="s">
-        <v>131</v>
+        <v>147</v>
       </c>
       <c r="D10" s="4"/>
     </row>
     <row r="11" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A11" s="4" t="s">
-        <v>132</v>
+        <v>148</v>
       </c>
       <c r="B11" s="4" t="s">
-        <v>128</v>
+        <v>144</v>
       </c>
       <c r="C11" s="4" t="s">
-        <v>133</v>
+        <v>149</v>
       </c>
       <c r="D11" s="4"/>
     </row>
     <row r="12" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A12" s="4" t="s">
-        <v>134</v>
+        <v>150</v>
       </c>
       <c r="B12" s="4" t="s">
-        <v>128</v>
+        <v>144</v>
       </c>
       <c r="C12" s="4" t="s">
-        <v>135</v>
+        <v>151</v>
       </c>
       <c r="D12" s="4"/>
     </row>
     <row r="13" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A13" s="4" t="s">
-        <v>136</v>
+        <v>152</v>
       </c>
       <c r="B13" s="4" t="s">
-        <v>128</v>
+        <v>144</v>
       </c>
       <c r="C13" s="4" t="s">
-        <v>137</v>
+        <v>153</v>
       </c>
       <c r="D13" s="4"/>
     </row>
     <row r="14" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A14" s="4" t="s">
-        <v>138</v>
+        <v>154</v>
       </c>
       <c r="B14" s="4" t="s">
-        <v>128</v>
+        <v>144</v>
       </c>
       <c r="C14" s="4" t="s">
-        <v>139</v>
+        <v>155</v>
       </c>
       <c r="D14" s="4"/>
     </row>
     <row r="15" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A15" s="4" t="s">
-        <v>140</v>
+        <v>156</v>
       </c>
       <c r="B15" s="4" t="s">
-        <v>128</v>
+        <v>144</v>
       </c>
       <c r="C15" s="4" t="s">
-        <v>141</v>
+        <v>157</v>
       </c>
       <c r="D15" s="4"/>
     </row>
     <row r="16" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A16" s="4" t="s">
-        <v>142</v>
+        <v>158</v>
       </c>
       <c r="B16" s="4" t="s">
-        <v>143</v>
+        <v>159</v>
       </c>
       <c r="C16" s="4" t="s">
-        <v>144</v>
+        <v>160</v>
       </c>
       <c r="D16" s="4"/>
     </row>
     <row r="17" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A17" s="4" t="s">
-        <v>145</v>
+        <v>161</v>
       </c>
       <c r="B17" s="4" t="s">
-        <v>143</v>
+        <v>159</v>
       </c>
       <c r="C17" s="4" t="s">
-        <v>146</v>
+        <v>162</v>
       </c>
       <c r="D17" s="4"/>
     </row>
     <row r="18" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A18" s="4" t="s">
-        <v>147</v>
+        <v>163</v>
       </c>
       <c r="B18" s="4" t="s">
-        <v>143</v>
+        <v>159</v>
       </c>
       <c r="C18" s="4" t="s">
-        <v>148</v>
+        <v>164</v>
       </c>
       <c r="D18" s="4"/>
     </row>
     <row r="19" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A19" s="4" t="s">
-        <v>149</v>
+        <v>165</v>
       </c>
       <c r="B19" s="4" t="s">
-        <v>143</v>
+        <v>159</v>
       </c>
       <c r="C19" s="4" t="s">
-        <v>150</v>
+        <v>166</v>
       </c>
       <c r="D19" s="4"/>
     </row>
     <row r="20" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A20" s="4" t="s">
-        <v>151</v>
+        <v>167</v>
       </c>
       <c r="B20" s="4" t="s">
-        <v>143</v>
+        <v>159</v>
       </c>
       <c r="C20" s="4" t="s">
-        <v>152</v>
+        <v>168</v>
       </c>
       <c r="D20" s="4"/>
     </row>
     <row r="21" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A21" s="4" t="s">
-        <v>153</v>
+        <v>169</v>
       </c>
       <c r="B21" s="4" t="s">
-        <v>143</v>
+        <v>159</v>
       </c>
       <c r="C21" s="4" t="s">
-        <v>154</v>
+        <v>170</v>
       </c>
       <c r="D21" s="4"/>
     </row>
     <row r="22" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A22" s="4" t="s">
-        <v>155</v>
+        <v>171</v>
       </c>
       <c r="B22" s="4" t="s">
-        <v>143</v>
+        <v>159</v>
       </c>
       <c r="C22" s="4" t="s">
-        <v>156</v>
+        <v>172</v>
       </c>
       <c r="D22" s="4"/>
     </row>
     <row r="23" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A23" s="4" t="s">
-        <v>157</v>
+        <v>173</v>
       </c>
       <c r="B23" s="4" t="s">
-        <v>158</v>
+        <v>174</v>
       </c>
       <c r="C23" s="4" t="s">
-        <v>159</v>
+        <v>175</v>
       </c>
       <c r="D23" s="4"/>
     </row>
     <row r="24" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A24" s="4" t="s">
-        <v>160</v>
+        <v>176</v>
       </c>
       <c r="B24" s="4" t="s">
-        <v>158</v>
+        <v>174</v>
       </c>
       <c r="C24" s="4" t="s">
-        <v>161</v>
+        <v>177</v>
       </c>
       <c r="D24" s="4"/>
     </row>
     <row r="25" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A25" s="4" t="s">
-        <v>162</v>
+        <v>178</v>
       </c>
       <c r="B25" s="4" t="s">
-        <v>158</v>
+        <v>174</v>
       </c>
       <c r="C25" s="4" t="s">
-        <v>163</v>
+        <v>179</v>
       </c>
       <c r="D25" s="4"/>
     </row>
     <row r="26" customFormat="false" ht="30" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A26" s="4" t="s">
-        <v>164</v>
+        <v>180</v>
       </c>
       <c r="B26" s="4" t="s">
-        <v>158</v>
+        <v>174</v>
       </c>
       <c r="C26" s="5" t="s">
-        <v>165</v>
+        <v>181</v>
       </c>
       <c r="D26" s="4"/>
     </row>
     <row r="27" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A27" s="4" t="s">
-        <v>166</v>
+        <v>182</v>
       </c>
       <c r="B27" s="4" t="s">
-        <v>158</v>
+        <v>174</v>
       </c>
       <c r="C27" s="4" t="s">
-        <v>167</v>
+        <v>183</v>
       </c>
       <c r="D27" s="4"/>
     </row>
     <row r="28" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A28" s="4" t="s">
-        <v>168</v>
+        <v>184</v>
       </c>
       <c r="B28" s="4" t="s">
-        <v>158</v>
+        <v>174</v>
       </c>
       <c r="C28" s="4" t="s">
-        <v>169</v>
+        <v>185</v>
       </c>
       <c r="D28" s="4"/>
     </row>
     <row r="29" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A29" s="4" t="s">
-        <v>170</v>
+        <v>186</v>
       </c>
       <c r="B29" s="4" t="s">
-        <v>158</v>
+        <v>174</v>
       </c>
       <c r="C29" s="4" t="s">
-        <v>171</v>
+        <v>187</v>
       </c>
       <c r="D29" s="4"/>
     </row>
     <row r="30" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A30" s="4" t="s">
-        <v>172</v>
+        <v>188</v>
       </c>
       <c r="B30" s="4" t="s">
-        <v>173</v>
+        <v>189</v>
       </c>
       <c r="C30" s="4" t="s">
-        <v>174</v>
+        <v>190</v>
       </c>
       <c r="D30" s="4"/>
     </row>
     <row r="31" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A31" s="4" t="s">
-        <v>175</v>
+        <v>191</v>
       </c>
       <c r="B31" s="4" t="s">
-        <v>173</v>
+        <v>189</v>
       </c>
       <c r="C31" s="4" t="s">
-        <v>176</v>
+        <v>192</v>
       </c>
       <c r="D31" s="4"/>
     </row>
     <row r="32" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A32" s="4" t="s">
-        <v>177</v>
+        <v>193</v>
       </c>
       <c r="B32" s="4" t="s">
-        <v>173</v>
+        <v>189</v>
       </c>
       <c r="C32" s="4" t="s">
-        <v>178</v>
+        <v>194</v>
       </c>
       <c r="D32" s="4"/>
     </row>
     <row r="33" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A33" s="4" t="s">
-        <v>179</v>
+        <v>195</v>
       </c>
       <c r="B33" s="4" t="s">
-        <v>173</v>
+        <v>189</v>
       </c>
       <c r="C33" s="4" t="s">
-        <v>180</v>
+        <v>196</v>
       </c>
       <c r="D33" s="4"/>
     </row>
     <row r="34" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A34" s="4" t="s">
-        <v>181</v>
+        <v>197</v>
       </c>
       <c r="B34" s="4" t="s">
-        <v>173</v>
+        <v>189</v>
       </c>
       <c r="C34" s="4" t="s">
-        <v>182</v>
+        <v>198</v>
       </c>
       <c r="D34" s="4"/>
     </row>
     <row r="35" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A35" s="4" t="s">
-        <v>183</v>
+        <v>199</v>
       </c>
       <c r="B35" s="4" t="s">
-        <v>173</v>
+        <v>189</v>
       </c>
       <c r="C35" s="4" t="s">
-        <v>184</v>
+        <v>200</v>
       </c>
       <c r="D35" s="4"/>
     </row>
     <row r="36" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A36" s="4" t="s">
-        <v>185</v>
+        <v>201</v>
       </c>
       <c r="B36" s="4" t="s">
-        <v>173</v>
+        <v>189</v>
       </c>
       <c r="C36" s="4" t="s">
-        <v>186</v>
+        <v>202</v>
       </c>
       <c r="D36" s="4"/>
     </row>
     <row r="37" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A37" s="4" t="s">
-        <v>187</v>
+        <v>203</v>
       </c>
       <c r="B37" s="4" t="s">
-        <v>188</v>
+        <v>204</v>
       </c>
       <c r="C37" s="4" t="s">
-        <v>189</v>
+        <v>205</v>
       </c>
       <c r="D37" s="4"/>
     </row>
     <row r="38" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A38" s="4" t="s">
-        <v>190</v>
+        <v>206</v>
       </c>
       <c r="B38" s="4" t="s">
-        <v>188</v>
+        <v>204</v>
       </c>
       <c r="C38" s="4" t="s">
-        <v>191</v>
+        <v>207</v>
       </c>
       <c r="D38" s="4"/>
     </row>
     <row r="39" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A39" s="4" t="s">
-        <v>192</v>
+        <v>208</v>
       </c>
       <c r="B39" s="4" t="s">
-        <v>188</v>
+        <v>204</v>
       </c>
       <c r="C39" s="4" t="s">
-        <v>193</v>
+        <v>209</v>
       </c>
       <c r="D39" s="4"/>
     </row>
     <row r="40" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A40" s="4" t="s">
-        <v>194</v>
+        <v>210</v>
       </c>
       <c r="B40" s="4" t="s">
-        <v>188</v>
+        <v>204</v>
       </c>
       <c r="C40" s="4" t="s">
-        <v>195</v>
+        <v>211</v>
       </c>
       <c r="D40" s="4"/>
     </row>
     <row r="41" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A41" s="4" t="s">
-        <v>196</v>
+        <v>212</v>
       </c>
       <c r="B41" s="4" t="s">
-        <v>188</v>
+        <v>204</v>
       </c>
       <c r="C41" s="4" t="s">
-        <v>197</v>
+        <v>213</v>
       </c>
       <c r="D41" s="4"/>
     </row>
     <row r="42" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A42" s="4" t="s">
-        <v>198</v>
+        <v>214</v>
       </c>
       <c r="B42" s="4" t="s">
-        <v>188</v>
+        <v>204</v>
       </c>
       <c r="C42" s="4" t="s">
-        <v>199</v>
+        <v>215</v>
       </c>
       <c r="D42" s="4"/>
     </row>
     <row r="43" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A43" s="4" t="s">
-        <v>200</v>
+        <v>216</v>
       </c>
       <c r="B43" s="4" t="s">
-        <v>188</v>
+        <v>204</v>
       </c>
       <c r="C43" s="4" t="s">
-        <v>201</v>
+        <v>217</v>
       </c>
       <c r="D43" s="4"/>
     </row>
@@ -4093,16 +4193,16 @@
   <sheetData>
     <row r="1" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A1" s="1" t="s">
-        <v>202</v>
+        <v>218</v>
       </c>
       <c r="B1" s="1" t="s">
-        <v>203</v>
+        <v>219</v>
       </c>
       <c r="C1" s="1" t="s">
-        <v>204</v>
+        <v>220</v>
       </c>
       <c r="D1" s="1" t="s">
-        <v>205</v>
+        <v>221</v>
       </c>
       <c r="E1" s="1"/>
     </row>
@@ -4346,16 +4446,16 @@
   <sheetData>
     <row r="1" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A1" s="1" t="s">
-        <v>206</v>
+        <v>222</v>
       </c>
       <c r="B1" s="1" t="s">
-        <v>207</v>
+        <v>223</v>
       </c>
       <c r="C1" s="1" t="s">
-        <v>208</v>
+        <v>224</v>
       </c>
       <c r="D1" s="1" t="s">
-        <v>209</v>
+        <v>225</v>
       </c>
       <c r="E1" s="1"/>
     </row>
@@ -4599,16 +4699,16 @@
   <sheetData>
     <row r="1" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A1" s="1" t="s">
-        <v>210</v>
+        <v>226</v>
       </c>
       <c r="B1" s="1" t="s">
-        <v>211</v>
+        <v>227</v>
       </c>
       <c r="C1" s="1" t="s">
-        <v>212</v>
+        <v>228</v>
       </c>
       <c r="D1" s="1" t="s">
-        <v>213</v>
+        <v>229</v>
       </c>
       <c r="E1" s="1"/>
     </row>
@@ -4852,7 +4952,7 @@
   <sheetData>
     <row r="1" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A1" s="1" t="s">
-        <v>214</v>
+        <v>230</v>
       </c>
       <c r="B1" s="1"/>
     </row>

</xml_diff>

<commit_message>
Added starting items based on choosing civ
</commit_message>
<xml_diff>
--- a/src/main/resources/assets/gamedata-faf-waw.xlsx
+++ b/src/main/resources/assets/gamedata-faf-waw.xlsx
@@ -5,7 +5,7 @@
   <workbookPr backupFile="false" showObjects="all" date1904="false"/>
   <workbookProtection/>
   <bookViews>
-    <workbookView showHorizontalScroll="true" showVerticalScroll="true" showSheetTabs="true" xWindow="0" yWindow="0" windowWidth="16384" windowHeight="8192" tabRatio="600" firstSheet="0" activeTab="17"/>
+    <workbookView showHorizontalScroll="true" showVerticalScroll="true" showSheetTabs="true" xWindow="0" yWindow="0" windowWidth="16384" windowHeight="8192" tabRatio="600" firstSheet="0" activeTab="0"/>
   </bookViews>
   <sheets>
     <sheet name="Civ" sheetId="1" state="visible" r:id="rId2"/>
@@ -166,7 +166,7 @@
     <t>Communism</t>
   </si>
   <si>
-    <t>The Russians start with 2 extra armies, and their stacking limit is increased by 1. Once per turn, the Russians maybe move an army or scout into an enemy city and sacrifice that figure to research a tech known by that civilization for free. Armies sacrificed this way cannot be also attack.</t>
+    <t>The Russians start with 2 armies, and their stacking limit is increased by 1. Once per turn, the Russians maybe move an army or scout into an enemy city and sacrifice that figure to research a tech known by that civilization for free. Armies sacrificed this way cannot be also attack.</t>
   </si>
   <si>
     <t>Spanish</t>
@@ -1274,7 +1274,7 @@
   </sheetPr>
   <dimension ref="A1:C17"/>
   <sheetViews>
-    <sheetView windowProtection="false" showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
+    <sheetView windowProtection="false" showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A4" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
       <selection pane="topLeft" activeCell="C17" activeCellId="0" sqref="C17"/>
     </sheetView>
   </sheetViews>
@@ -2815,7 +2815,7 @@
   </sheetPr>
   <dimension ref="A1:B10"/>
   <sheetViews>
-    <sheetView windowProtection="false" showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
+    <sheetView windowProtection="false" showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
       <selection pane="topLeft" activeCell="A9" activeCellId="0" sqref="A9"/>
     </sheetView>
   </sheetViews>

</xml_diff>

<commit_message>
Added support for anarchy lvl 1
</commit_message>
<xml_diff>
--- a/src/main/resources/assets/gamedata-faf-waw.xlsx
+++ b/src/main/resources/assets/gamedata-faf-waw.xlsx
@@ -5,7 +5,7 @@
   <workbookPr backupFile="false" showObjects="all" date1904="false"/>
   <workbookProtection/>
   <bookViews>
-    <workbookView showHorizontalScroll="true" showVerticalScroll="true" showSheetTabs="true" xWindow="0" yWindow="0" windowWidth="16384" windowHeight="8192" tabRatio="600" firstSheet="0" activeTab="18"/>
+    <workbookView showHorizontalScroll="true" showVerticalScroll="true" showSheetTabs="true" xWindow="0" yWindow="0" windowWidth="16384" windowHeight="8192" tabRatio="600" firstSheet="0" activeTab="2"/>
   </bookViews>
   <sheets>
     <sheet name="Civ" sheetId="1" state="visible" r:id="rId2"/>
@@ -33,7 +33,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="574" uniqueCount="385">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="574" uniqueCount="386">
   <si>
     <t>Civilization</t>
   </si>
@@ -339,6 +339,9 @@
   </si>
   <si>
     <t>Movement : Choose an army figure or city token within four squares (no diagonals) of a village token or revealed village icon. That figure or city is immediately attacked by rank II barbarians.</t>
+  </si>
+  <si>
+    <t>The Citizens are Revolting II!</t>
   </si>
   <si>
     <t>We Love the Queen Day!</t>
@@ -1555,108 +1558,108 @@
   <sheetData>
     <row r="1" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A1" s="1" t="s">
-        <v>231</v>
+        <v>232</v>
       </c>
       <c r="B1" s="1"/>
     </row>
     <row r="2" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A2" s="0" t="s">
-        <v>232</v>
+        <v>233</v>
       </c>
     </row>
     <row r="3" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A3" s="0" t="s">
-        <v>232</v>
+        <v>233</v>
       </c>
     </row>
     <row r="4" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A4" s="0" t="s">
-        <v>232</v>
+        <v>233</v>
       </c>
     </row>
     <row r="5" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A5" s="0" t="s">
-        <v>233</v>
+        <v>234</v>
       </c>
     </row>
     <row r="6" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A6" s="0" t="s">
-        <v>234</v>
+        <v>235</v>
       </c>
     </row>
     <row r="7" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A7" s="0" t="s">
-        <v>234</v>
+        <v>235</v>
       </c>
     </row>
     <row r="8" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A8" s="0" t="s">
-        <v>235</v>
+        <v>236</v>
       </c>
     </row>
     <row r="9" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A9" s="0" t="s">
-        <v>235</v>
+        <v>236</v>
       </c>
     </row>
     <row r="10" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A10" s="0" t="s">
-        <v>235</v>
+        <v>236</v>
       </c>
     </row>
     <row r="11" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A11" s="0" t="s">
-        <v>236</v>
+        <v>237</v>
       </c>
     </row>
     <row r="12" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A12" s="0" t="s">
-        <v>237</v>
+        <v>238</v>
       </c>
     </row>
     <row r="13" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A13" s="0" t="s">
-        <v>237</v>
+        <v>238</v>
       </c>
     </row>
     <row r="14" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A14" s="0" t="s">
-        <v>237</v>
+        <v>238</v>
       </c>
     </row>
     <row r="15" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A15" s="0" t="s">
-        <v>237</v>
+        <v>238</v>
       </c>
     </row>
     <row r="16" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A16" s="0" t="s">
-        <v>238</v>
+        <v>239</v>
       </c>
     </row>
     <row r="17" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A17" s="0" t="s">
-        <v>238</v>
+        <v>239</v>
       </c>
     </row>
     <row r="18" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A18" s="0" t="s">
-        <v>238</v>
+        <v>239</v>
       </c>
     </row>
     <row r="19" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A19" s="0" t="s">
-        <v>238</v>
+        <v>239</v>
       </c>
     </row>
     <row r="20" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A20" s="0" t="s">
-        <v>239</v>
+        <v>240</v>
       </c>
     </row>
     <row r="21" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A21" s="0" t="s">
-        <v>239</v>
+        <v>240</v>
       </c>
     </row>
   </sheetData>
@@ -1690,183 +1693,183 @@
   <sheetData>
     <row r="1" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A1" s="1" t="s">
-        <v>240</v>
+        <v>241</v>
       </c>
       <c r="B1" s="1"/>
     </row>
     <row r="2" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A2" s="0" t="s">
-        <v>232</v>
+        <v>233</v>
       </c>
     </row>
     <row r="3" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A3" s="0" t="s">
-        <v>232</v>
+        <v>233</v>
       </c>
     </row>
     <row r="4" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A4" s="0" t="s">
-        <v>241</v>
+        <v>242</v>
       </c>
     </row>
     <row r="5" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A5" s="0" t="s">
-        <v>241</v>
+        <v>242</v>
       </c>
     </row>
     <row r="6" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A6" s="0" t="s">
-        <v>242</v>
+        <v>243</v>
       </c>
     </row>
     <row r="7" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A7" s="0" t="s">
-        <v>242</v>
+        <v>243</v>
       </c>
     </row>
     <row r="8" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A8" s="0" t="s">
-        <v>242</v>
+        <v>243</v>
       </c>
     </row>
     <row r="9" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A9" s="0" t="s">
-        <v>242</v>
+        <v>243</v>
       </c>
     </row>
     <row r="10" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A10" s="0" t="s">
-        <v>242</v>
+        <v>243</v>
       </c>
     </row>
     <row r="11" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A11" s="0" t="s">
-        <v>242</v>
+        <v>243</v>
       </c>
     </row>
     <row r="12" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A12" s="0" t="s">
-        <v>235</v>
+        <v>236</v>
       </c>
     </row>
     <row r="13" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A13" s="0" t="s">
-        <v>235</v>
+        <v>236</v>
       </c>
     </row>
     <row r="14" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A14" s="0" t="s">
-        <v>235</v>
+        <v>236</v>
       </c>
     </row>
     <row r="15" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A15" s="0" t="s">
-        <v>243</v>
+        <v>244</v>
       </c>
     </row>
     <row r="16" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A16" s="0" t="s">
-        <v>244</v>
+        <v>245</v>
       </c>
     </row>
     <row r="17" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A17" s="0" t="s">
-        <v>244</v>
+        <v>245</v>
       </c>
     </row>
     <row r="18" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A18" s="0" t="s">
-        <v>244</v>
+        <v>245</v>
       </c>
     </row>
     <row r="19" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A19" s="0" t="s">
-        <v>244</v>
+        <v>245</v>
       </c>
     </row>
     <row r="20" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A20" s="0" t="s">
-        <v>244</v>
+        <v>245</v>
       </c>
     </row>
     <row r="21" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A21" s="0" t="s">
-        <v>244</v>
+        <v>245</v>
       </c>
     </row>
     <row r="22" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A22" s="0" t="s">
-        <v>237</v>
+        <v>238</v>
       </c>
     </row>
     <row r="23" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A23" s="0" t="s">
-        <v>237</v>
+        <v>238</v>
       </c>
     </row>
     <row r="24" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A24" s="0" t="s">
-        <v>237</v>
+        <v>238</v>
       </c>
     </row>
     <row r="25" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A25" s="0" t="s">
-        <v>237</v>
+        <v>238</v>
       </c>
     </row>
     <row r="26" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A26" s="0" t="s">
-        <v>237</v>
+        <v>238</v>
       </c>
     </row>
     <row r="27" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A27" s="0" t="s">
-        <v>237</v>
+        <v>238</v>
       </c>
     </row>
     <row r="28" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A28" s="0" t="s">
-        <v>245</v>
+        <v>246</v>
       </c>
     </row>
     <row r="29" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A29" s="0" t="s">
-        <v>238</v>
+        <v>239</v>
       </c>
     </row>
     <row r="30" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A30" s="0" t="s">
-        <v>246</v>
+        <v>247</v>
       </c>
     </row>
     <row r="31" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A31" s="0" t="s">
-        <v>246</v>
+        <v>247</v>
       </c>
     </row>
     <row r="32" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A32" s="0" t="s">
-        <v>246</v>
+        <v>247</v>
       </c>
     </row>
     <row r="33" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A33" s="0" t="s">
-        <v>246</v>
+        <v>247</v>
       </c>
     </row>
     <row r="34" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A34" s="0" t="s">
-        <v>246</v>
+        <v>247</v>
       </c>
     </row>
     <row r="35" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A35" s="0" t="s">
-        <v>246</v>
+        <v>247</v>
       </c>
     </row>
     <row r="36" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A36" s="0" t="s">
-        <v>246</v>
+        <v>247</v>
       </c>
     </row>
   </sheetData>
@@ -1903,39 +1906,39 @@
   <sheetData>
     <row r="1" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A1" s="1" t="s">
-        <v>247</v>
+        <v>248</v>
       </c>
       <c r="B1" s="1" t="s">
         <v>2</v>
       </c>
       <c r="C1" s="1" t="s">
-        <v>248</v>
+        <v>249</v>
       </c>
       <c r="D1" s="1" t="s">
-        <v>249</v>
+        <v>250</v>
       </c>
       <c r="E1" s="1"/>
     </row>
     <row r="2" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A2" s="0" t="s">
-        <v>250</v>
+        <v>251</v>
       </c>
       <c r="B2" s="0" t="s">
-        <v>251</v>
+        <v>252</v>
       </c>
       <c r="C2" s="0" t="n">
         <v>15</v>
       </c>
       <c r="D2" s="0" t="s">
-        <v>252</v>
+        <v>253</v>
       </c>
     </row>
     <row r="3" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A3" s="0" t="s">
-        <v>253</v>
+        <v>254</v>
       </c>
       <c r="B3" s="0" t="s">
-        <v>254</v>
+        <v>255</v>
       </c>
       <c r="C3" s="0" t="n">
         <v>15</v>
@@ -1943,10 +1946,10 @@
     </row>
     <row r="4" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A4" s="0" t="s">
-        <v>255</v>
+        <v>256</v>
       </c>
       <c r="B4" s="0" t="s">
-        <v>256</v>
+        <v>257</v>
       </c>
       <c r="C4" s="0" t="n">
         <v>10</v>
@@ -1954,123 +1957,123 @@
     </row>
     <row r="5" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A5" s="0" t="s">
-        <v>257</v>
+        <v>258</v>
       </c>
       <c r="B5" s="0" t="s">
-        <v>258</v>
+        <v>259</v>
       </c>
       <c r="C5" s="0" t="n">
         <v>15</v>
       </c>
       <c r="D5" s="0" t="s">
-        <v>259</v>
+        <v>260</v>
       </c>
     </row>
     <row r="6" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A6" s="0" t="s">
-        <v>260</v>
+        <v>261</v>
       </c>
       <c r="B6" s="0" t="s">
-        <v>261</v>
+        <v>262</v>
       </c>
       <c r="C6" s="0" t="n">
         <v>15</v>
       </c>
       <c r="D6" s="0" t="s">
-        <v>262</v>
+        <v>263</v>
       </c>
     </row>
     <row r="7" customFormat="false" ht="30" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A7" s="0" t="s">
-        <v>263</v>
+        <v>264</v>
       </c>
       <c r="B7" s="5" t="s">
-        <v>264</v>
+        <v>265</v>
       </c>
       <c r="C7" s="0" t="n">
         <v>15</v>
       </c>
       <c r="D7" s="0" t="s">
-        <v>265</v>
+        <v>266</v>
       </c>
     </row>
     <row r="8" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A8" s="0" t="s">
-        <v>266</v>
+        <v>267</v>
       </c>
       <c r="B8" s="0" t="s">
-        <v>267</v>
+        <v>268</v>
       </c>
       <c r="C8" s="0" t="n">
         <v>15</v>
       </c>
       <c r="D8" s="0" t="s">
-        <v>268</v>
+        <v>269</v>
       </c>
     </row>
     <row r="9" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A9" s="0" t="s">
-        <v>269</v>
+        <v>270</v>
       </c>
       <c r="B9" s="0" t="s">
-        <v>270</v>
+        <v>271</v>
       </c>
       <c r="C9" s="0" t="n">
         <v>15</v>
       </c>
       <c r="D9" s="0" t="s">
-        <v>271</v>
+        <v>272</v>
       </c>
     </row>
     <row r="10" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A10" s="0" t="s">
-        <v>272</v>
+        <v>273</v>
       </c>
       <c r="B10" s="0" t="s">
-        <v>273</v>
+        <v>274</v>
       </c>
       <c r="C10" s="0" t="n">
         <v>15</v>
       </c>
       <c r="D10" s="0" t="s">
-        <v>274</v>
+        <v>275</v>
       </c>
     </row>
     <row r="12" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A12" s="1" t="s">
-        <v>275</v>
+        <v>276</v>
       </c>
       <c r="B12" s="1" t="s">
         <v>2</v>
       </c>
       <c r="C12" s="1" t="s">
-        <v>248</v>
+        <v>249</v>
       </c>
       <c r="D12" s="1" t="s">
-        <v>249</v>
+        <v>250</v>
       </c>
       <c r="E12" s="1"/>
     </row>
     <row r="13" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A13" s="0" t="s">
-        <v>276</v>
+        <v>277</v>
       </c>
       <c r="B13" s="0" t="s">
-        <v>277</v>
+        <v>278</v>
       </c>
       <c r="C13" s="0" t="n">
         <v>20</v>
       </c>
       <c r="D13" s="0" t="s">
-        <v>278</v>
+        <v>279</v>
       </c>
     </row>
     <row r="14" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A14" s="0" t="s">
-        <v>279</v>
+        <v>280</v>
       </c>
       <c r="B14" s="0" t="s">
-        <v>280</v>
+        <v>281</v>
       </c>
       <c r="C14" s="0" t="n">
         <v>15</v>
@@ -2078,179 +2081,179 @@
     </row>
     <row r="15" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A15" s="0" t="s">
-        <v>281</v>
+        <v>282</v>
       </c>
       <c r="B15" s="0" t="s">
-        <v>282</v>
+        <v>283</v>
       </c>
       <c r="C15" s="0" t="n">
         <v>20</v>
       </c>
       <c r="D15" s="0" t="s">
-        <v>283</v>
+        <v>284</v>
       </c>
     </row>
     <row r="16" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A16" s="0" t="s">
-        <v>284</v>
+        <v>285</v>
       </c>
       <c r="B16" s="0" t="s">
-        <v>285</v>
+        <v>286</v>
       </c>
       <c r="C16" s="0" t="n">
         <v>20</v>
       </c>
       <c r="D16" s="0" t="s">
-        <v>286</v>
+        <v>287</v>
       </c>
     </row>
     <row r="17" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A17" s="0" t="s">
-        <v>287</v>
+        <v>288</v>
       </c>
       <c r="B17" s="0" t="s">
-        <v>288</v>
+        <v>289</v>
       </c>
       <c r="C17" s="0" t="n">
         <v>20</v>
       </c>
       <c r="D17" s="0" t="s">
-        <v>289</v>
+        <v>290</v>
       </c>
     </row>
     <row r="18" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A18" s="0" t="s">
-        <v>290</v>
+        <v>291</v>
       </c>
       <c r="B18" s="0" t="s">
-        <v>291</v>
+        <v>292</v>
       </c>
       <c r="C18" s="0" t="n">
         <v>20</v>
       </c>
       <c r="D18" s="0" t="s">
-        <v>292</v>
+        <v>293</v>
       </c>
     </row>
     <row r="19" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A19" s="0" t="s">
-        <v>293</v>
+        <v>294</v>
       </c>
       <c r="B19" s="0" t="s">
-        <v>294</v>
+        <v>295</v>
       </c>
       <c r="C19" s="0" t="n">
         <v>20</v>
       </c>
       <c r="D19" s="0" t="s">
-        <v>295</v>
+        <v>296</v>
       </c>
     </row>
     <row r="20" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A20" s="0" t="s">
-        <v>296</v>
+        <v>297</v>
       </c>
       <c r="B20" s="0" t="s">
-        <v>297</v>
+        <v>298</v>
       </c>
       <c r="C20" s="0" t="n">
         <v>20</v>
       </c>
       <c r="D20" s="0" t="s">
-        <v>298</v>
+        <v>299</v>
       </c>
     </row>
     <row r="21" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A21" s="0" t="s">
-        <v>299</v>
+        <v>300</v>
       </c>
       <c r="B21" s="0" t="s">
-        <v>300</v>
+        <v>301</v>
       </c>
       <c r="C21" s="0" t="n">
         <v>20</v>
       </c>
       <c r="D21" s="0" t="s">
-        <v>301</v>
+        <v>302</v>
       </c>
     </row>
     <row r="23" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A23" s="1" t="s">
-        <v>302</v>
+        <v>303</v>
       </c>
       <c r="B23" s="1" t="s">
         <v>2</v>
       </c>
       <c r="C23" s="1" t="s">
-        <v>248</v>
+        <v>249</v>
       </c>
       <c r="D23" s="1" t="s">
-        <v>249</v>
+        <v>250</v>
       </c>
       <c r="E23" s="1"/>
     </row>
     <row r="24" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A24" s="0" t="s">
-        <v>303</v>
+        <v>304</v>
       </c>
       <c r="B24" s="0" t="s">
-        <v>304</v>
+        <v>305</v>
       </c>
       <c r="C24" s="0" t="n">
         <v>25</v>
       </c>
       <c r="D24" s="0" t="s">
-        <v>305</v>
+        <v>306</v>
       </c>
     </row>
     <row r="25" customFormat="false" ht="30" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A25" s="0" t="s">
-        <v>306</v>
+        <v>307</v>
       </c>
       <c r="B25" s="5" t="s">
-        <v>307</v>
+        <v>308</v>
       </c>
       <c r="C25" s="0" t="n">
         <v>25</v>
       </c>
       <c r="D25" s="0" t="s">
-        <v>308</v>
+        <v>309</v>
       </c>
     </row>
     <row r="26" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A26" s="0" t="s">
-        <v>309</v>
+        <v>310</v>
       </c>
       <c r="B26" s="0" t="s">
-        <v>310</v>
+        <v>311</v>
       </c>
       <c r="C26" s="0" t="n">
         <v>25</v>
       </c>
       <c r="D26" s="0" t="s">
-        <v>311</v>
+        <v>312</v>
       </c>
     </row>
     <row r="27" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A27" s="0" t="s">
-        <v>312</v>
+        <v>313</v>
       </c>
       <c r="B27" s="0" t="s">
-        <v>313</v>
+        <v>314</v>
       </c>
       <c r="C27" s="0" t="n">
         <v>25</v>
       </c>
       <c r="D27" s="0" t="s">
-        <v>314</v>
+        <v>315</v>
       </c>
     </row>
     <row r="28" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A28" s="0" t="s">
-        <v>315</v>
+        <v>316</v>
       </c>
       <c r="B28" s="0" t="s">
-        <v>316</v>
+        <v>317</v>
       </c>
       <c r="C28" s="0" t="n">
         <v>25</v>
@@ -2258,52 +2261,52 @@
     </row>
     <row r="29" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A29" s="0" t="s">
-        <v>317</v>
+        <v>318</v>
       </c>
       <c r="B29" s="0" t="s">
-        <v>318</v>
+        <v>319</v>
       </c>
       <c r="C29" s="0" t="n">
         <v>25</v>
       </c>
       <c r="D29" s="0" t="s">
-        <v>319</v>
+        <v>320</v>
       </c>
     </row>
     <row r="30" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A30" s="0" t="s">
-        <v>320</v>
+        <v>321</v>
       </c>
       <c r="B30" s="0" t="s">
-        <v>321</v>
+        <v>322</v>
       </c>
       <c r="C30" s="0" t="n">
         <v>25</v>
       </c>
       <c r="D30" s="0" t="s">
-        <v>322</v>
+        <v>323</v>
       </c>
     </row>
     <row r="31" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A31" s="0" t="s">
-        <v>323</v>
+        <v>324</v>
       </c>
       <c r="B31" s="0" t="s">
-        <v>324</v>
+        <v>325</v>
       </c>
       <c r="C31" s="0" t="n">
         <v>25</v>
       </c>
       <c r="D31" s="0" t="s">
-        <v>325</v>
+        <v>326</v>
       </c>
     </row>
     <row r="32" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A32" s="0" t="s">
-        <v>326</v>
+        <v>327</v>
       </c>
       <c r="B32" s="0" t="s">
-        <v>327</v>
+        <v>328</v>
       </c>
       <c r="C32" s="0" t="n">
         <v>20</v>
@@ -2339,7 +2342,7 @@
   <sheetData>
     <row r="1" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A1" s="1" t="s">
-        <v>127</v>
+        <v>128</v>
       </c>
       <c r="B1" s="1"/>
     </row>
@@ -2510,7 +2513,7 @@
   <sheetData>
     <row r="1" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A1" s="1" t="s">
-        <v>328</v>
+        <v>329</v>
       </c>
       <c r="B1" s="1" t="s">
         <v>2</v>
@@ -2518,42 +2521,42 @@
     </row>
     <row r="2" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A2" s="0" t="s">
-        <v>329</v>
+        <v>330</v>
       </c>
       <c r="B2" s="0" t="s">
-        <v>330</v>
+        <v>331</v>
       </c>
     </row>
     <row r="3" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A3" s="0" t="s">
-        <v>331</v>
+        <v>332</v>
       </c>
       <c r="B3" s="0" t="s">
-        <v>332</v>
+        <v>333</v>
       </c>
     </row>
     <row r="4" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A4" s="0" t="s">
-        <v>333</v>
+        <v>334</v>
       </c>
       <c r="B4" s="0" t="s">
-        <v>334</v>
+        <v>335</v>
       </c>
     </row>
     <row r="5" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A5" s="0" t="s">
-        <v>335</v>
+        <v>336</v>
       </c>
       <c r="B5" s="0" t="s">
-        <v>336</v>
+        <v>337</v>
       </c>
     </row>
     <row r="6" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A6" s="0" t="s">
-        <v>337</v>
+        <v>338</v>
       </c>
       <c r="B6" s="0" t="s">
-        <v>338</v>
+        <v>339</v>
       </c>
     </row>
     <row r="16" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
@@ -2591,7 +2594,7 @@
   <sheetData>
     <row r="1" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A1" s="1" t="s">
-        <v>339</v>
+        <v>340</v>
       </c>
       <c r="B1" s="1" t="s">
         <v>2</v>
@@ -2624,7 +2627,7 @@
     </row>
     <row r="7" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A7" s="0" t="s">
-        <v>340</v>
+        <v>341</v>
       </c>
     </row>
     <row r="8" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -2639,7 +2642,7 @@
     </row>
     <row r="10" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A10" s="0" t="s">
-        <v>341</v>
+        <v>342</v>
       </c>
     </row>
     <row r="11" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -2687,7 +2690,7 @@
   <sheetData>
     <row r="1" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A1" s="1" t="s">
-        <v>339</v>
+        <v>340</v>
       </c>
       <c r="B1" s="1" t="s">
         <v>2</v>
@@ -2695,7 +2698,7 @@
     </row>
     <row r="2" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A2" s="0" t="s">
-        <v>342</v>
+        <v>343</v>
       </c>
     </row>
     <row r="3" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -2715,7 +2718,7 @@
     </row>
     <row r="6" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A6" s="0" t="s">
-        <v>343</v>
+        <v>344</v>
       </c>
     </row>
     <row r="7" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -2730,32 +2733,32 @@
     </row>
     <row r="9" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A9" s="0" t="s">
-        <v>344</v>
+        <v>345</v>
       </c>
     </row>
     <row r="10" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A10" s="0" t="s">
-        <v>345</v>
+        <v>346</v>
       </c>
     </row>
     <row r="11" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A11" s="0" t="s">
-        <v>346</v>
+        <v>347</v>
       </c>
     </row>
     <row r="12" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A12" s="0" t="s">
-        <v>347</v>
+        <v>348</v>
       </c>
     </row>
     <row r="13" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A13" s="0" t="s">
-        <v>348</v>
+        <v>349</v>
       </c>
     </row>
     <row r="14" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A14" s="0" t="s">
-        <v>349</v>
+        <v>350</v>
       </c>
     </row>
   </sheetData>
@@ -2788,7 +2791,7 @@
   <sheetData>
     <row r="1" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A1" s="1" t="s">
-        <v>339</v>
+        <v>340</v>
       </c>
       <c r="B1" s="1" t="s">
         <v>2</v>
@@ -2796,12 +2799,12 @@
     </row>
     <row r="2" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A2" s="0" t="s">
-        <v>350</v>
+        <v>351</v>
       </c>
     </row>
     <row r="3" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A3" s="0" t="s">
-        <v>351</v>
+        <v>352</v>
       </c>
     </row>
     <row r="4" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -2811,42 +2814,42 @@
     </row>
     <row r="5" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A5" s="0" t="s">
-        <v>352</v>
+        <v>353</v>
       </c>
     </row>
     <row r="6" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A6" s="0" t="s">
-        <v>353</v>
+        <v>354</v>
       </c>
     </row>
     <row r="7" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A7" s="0" t="s">
-        <v>354</v>
+        <v>355</v>
       </c>
     </row>
     <row r="8" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A8" s="0" t="s">
-        <v>355</v>
+        <v>356</v>
       </c>
     </row>
     <row r="9" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A9" s="0" t="s">
-        <v>356</v>
+        <v>357</v>
       </c>
     </row>
     <row r="10" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A10" s="0" t="s">
-        <v>357</v>
+        <v>358</v>
       </c>
     </row>
     <row r="11" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A11" s="0" t="s">
-        <v>358</v>
+        <v>359</v>
       </c>
     </row>
     <row r="12" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A12" s="0" t="s">
-        <v>359</v>
+        <v>360</v>
       </c>
     </row>
   </sheetData>
@@ -2879,7 +2882,7 @@
   <sheetData>
     <row r="1" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A1" s="1" t="s">
-        <v>339</v>
+        <v>340</v>
       </c>
       <c r="B1" s="1" t="s">
         <v>2</v>
@@ -2887,42 +2890,42 @@
     </row>
     <row r="2" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A2" s="0" t="s">
-        <v>360</v>
+        <v>361</v>
       </c>
     </row>
     <row r="3" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A3" s="0" t="s">
-        <v>361</v>
+        <v>362</v>
       </c>
     </row>
     <row r="4" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A4" s="0" t="s">
-        <v>362</v>
+        <v>363</v>
       </c>
     </row>
     <row r="5" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A5" s="0" t="s">
-        <v>363</v>
+        <v>364</v>
       </c>
     </row>
     <row r="6" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A6" s="0" t="s">
-        <v>364</v>
+        <v>365</v>
       </c>
     </row>
     <row r="7" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A7" s="0" t="s">
-        <v>365</v>
+        <v>366</v>
       </c>
     </row>
     <row r="8" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A8" s="0" t="s">
-        <v>366</v>
+        <v>367</v>
       </c>
     </row>
     <row r="9" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A9" s="0" t="s">
-        <v>367</v>
+        <v>368</v>
       </c>
     </row>
     <row r="10" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
@@ -2945,7 +2948,7 @@
   </sheetPr>
   <dimension ref="A1:C9"/>
   <sheetViews>
-    <sheetView windowProtection="false" showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
+    <sheetView windowProtection="false" showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
       <selection pane="topLeft" activeCell="E27" activeCellId="0" sqref="E27"/>
     </sheetView>
   </sheetViews>
@@ -2959,101 +2962,101 @@
   <sheetData>
     <row r="1" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A1" s="1" t="s">
-        <v>339</v>
+        <v>340</v>
       </c>
       <c r="B1" s="1" t="s">
         <v>2</v>
       </c>
       <c r="C1" s="1" t="s">
-        <v>368</v>
+        <v>369</v>
       </c>
     </row>
     <row r="2" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A2" s="0" t="s">
-        <v>369</v>
+        <v>370</v>
       </c>
       <c r="B2" s="0" t="s">
-        <v>370</v>
+        <v>371</v>
       </c>
       <c r="C2" s="0" t="s">
-        <v>371</v>
+        <v>372</v>
       </c>
     </row>
     <row r="3" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A3" s="0" t="s">
-        <v>372</v>
+        <v>373</v>
       </c>
       <c r="B3" s="0" t="s">
-        <v>373</v>
+        <v>374</v>
       </c>
       <c r="C3" s="0" t="s">
-        <v>374</v>
+        <v>375</v>
       </c>
     </row>
     <row r="4" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A4" s="0" t="s">
-        <v>375</v>
+        <v>376</v>
       </c>
       <c r="B4" s="0" t="s">
-        <v>376</v>
+        <v>377</v>
       </c>
       <c r="C4" s="0" t="s">
-        <v>377</v>
+        <v>378</v>
       </c>
     </row>
     <row r="5" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A5" s="0" t="s">
-        <v>378</v>
+        <v>379</v>
       </c>
       <c r="B5" s="0" t="s">
-        <v>379</v>
+        <v>380</v>
       </c>
       <c r="C5" s="0" t="s">
-        <v>380</v>
+        <v>381</v>
       </c>
     </row>
     <row r="6" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A6" s="0" t="s">
-        <v>371</v>
+        <v>372</v>
       </c>
       <c r="B6" s="0" t="s">
-        <v>381</v>
+        <v>382</v>
       </c>
       <c r="C6" s="0" t="s">
-        <v>369</v>
+        <v>370</v>
       </c>
     </row>
     <row r="7" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A7" s="0" t="s">
-        <v>374</v>
+        <v>375</v>
       </c>
       <c r="B7" s="0" t="s">
-        <v>382</v>
+        <v>383</v>
       </c>
       <c r="C7" s="0" t="s">
-        <v>372</v>
+        <v>373</v>
       </c>
     </row>
     <row r="8" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A8" s="0" t="s">
-        <v>377</v>
+        <v>378</v>
       </c>
       <c r="B8" s="0" t="s">
-        <v>383</v>
+        <v>384</v>
       </c>
       <c r="C8" s="0" t="s">
-        <v>375</v>
+        <v>376</v>
       </c>
     </row>
     <row r="9" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A9" s="0" t="s">
-        <v>380</v>
+        <v>381</v>
       </c>
       <c r="B9" s="0" t="s">
-        <v>384</v>
+        <v>385</v>
       </c>
       <c r="C9" s="0" t="s">
-        <v>371</v>
+        <v>372</v>
       </c>
     </row>
   </sheetData>
@@ -3075,7 +3078,7 @@
   <dimension ref="A1:C28"/>
   <sheetViews>
     <sheetView windowProtection="false" showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="C1" activeCellId="0" sqref="C1"/>
+      <selection pane="topLeft" activeCell="A25" activeCellId="0" sqref="A25"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15"/>
@@ -3355,8 +3358,8 @@
   </sheetPr>
   <dimension ref="A1:C26"/>
   <sheetViews>
-    <sheetView windowProtection="false" showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="C1" activeCellId="0" sqref="C1"/>
+    <sheetView windowProtection="false" showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
+      <selection pane="topLeft" activeCell="A25" activeCellId="0" sqref="A25"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15"/>
@@ -3575,7 +3578,7 @@
     </row>
     <row r="24" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A24" s="2" t="s">
-        <v>74</v>
+        <v>102</v>
       </c>
       <c r="B24" s="2" t="s">
         <v>75</v>
@@ -3584,19 +3587,19 @@
     </row>
     <row r="25" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A25" s="2" t="s">
-        <v>102</v>
+        <v>103</v>
       </c>
       <c r="B25" s="2" t="s">
-        <v>103</v>
+        <v>104</v>
       </c>
       <c r="C25" s="2"/>
     </row>
     <row r="26" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A26" s="2" t="s">
-        <v>102</v>
+        <v>103</v>
       </c>
       <c r="B26" s="2" t="s">
-        <v>103</v>
+        <v>104</v>
       </c>
       <c r="C26" s="2"/>
     </row>
@@ -3640,154 +3643,154 @@
     </row>
     <row r="2" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A2" s="2" t="s">
-        <v>104</v>
+        <v>105</v>
       </c>
       <c r="B2" s="2" t="s">
-        <v>105</v>
+        <v>106</v>
       </c>
       <c r="C2" s="2"/>
     </row>
     <row r="3" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A3" s="2" t="s">
-        <v>104</v>
+        <v>105</v>
       </c>
       <c r="B3" s="2" t="s">
-        <v>105</v>
+        <v>106</v>
       </c>
       <c r="C3" s="2"/>
     </row>
     <row r="4" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A4" s="2" t="s">
-        <v>106</v>
+        <v>107</v>
       </c>
       <c r="B4" s="2" t="s">
-        <v>107</v>
+        <v>108</v>
       </c>
       <c r="C4" s="2"/>
     </row>
     <row r="5" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A5" s="2" t="s">
-        <v>108</v>
+        <v>109</v>
       </c>
       <c r="B5" s="2" t="s">
-        <v>109</v>
+        <v>110</v>
       </c>
       <c r="C5" s="2"/>
     </row>
     <row r="6" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A6" s="2" t="s">
-        <v>110</v>
+        <v>111</v>
       </c>
       <c r="B6" s="2" t="s">
-        <v>111</v>
+        <v>112</v>
       </c>
       <c r="C6" s="2"/>
     </row>
     <row r="7" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A7" s="2" t="s">
-        <v>110</v>
+        <v>111</v>
       </c>
       <c r="B7" s="2" t="s">
-        <v>111</v>
+        <v>112</v>
       </c>
       <c r="C7" s="2"/>
     </row>
     <row r="8" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A8" s="2" t="s">
-        <v>112</v>
+        <v>113</v>
       </c>
       <c r="B8" s="2" t="s">
-        <v>113</v>
+        <v>114</v>
       </c>
       <c r="C8" s="2"/>
     </row>
     <row r="9" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A9" s="2" t="s">
-        <v>114</v>
+        <v>115</v>
       </c>
       <c r="B9" s="2" t="s">
-        <v>115</v>
+        <v>116</v>
       </c>
       <c r="C9" s="2"/>
     </row>
     <row r="10" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A10" s="2" t="s">
-        <v>116</v>
+        <v>117</v>
       </c>
       <c r="B10" s="2" t="s">
-        <v>117</v>
+        <v>118</v>
       </c>
       <c r="C10" s="2"/>
     </row>
     <row r="11" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A11" s="2" t="s">
-        <v>116</v>
+        <v>117</v>
       </c>
       <c r="B11" s="2" t="s">
-        <v>117</v>
+        <v>118</v>
       </c>
       <c r="C11" s="2"/>
     </row>
     <row r="12" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A12" s="2" t="s">
-        <v>118</v>
+        <v>119</v>
       </c>
       <c r="B12" s="2" t="s">
-        <v>119</v>
+        <v>120</v>
       </c>
       <c r="C12" s="2"/>
     </row>
     <row r="13" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A13" s="2" t="s">
-        <v>118</v>
+        <v>119</v>
       </c>
       <c r="B13" s="2" t="s">
-        <v>119</v>
+        <v>120</v>
       </c>
       <c r="C13" s="2"/>
     </row>
     <row r="14" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A14" s="2" t="s">
-        <v>120</v>
+        <v>121</v>
       </c>
       <c r="B14" s="2" t="s">
-        <v>121</v>
+        <v>122</v>
       </c>
       <c r="C14" s="2"/>
     </row>
     <row r="15" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A15" s="2" t="s">
-        <v>120</v>
+        <v>121</v>
       </c>
       <c r="B15" s="2" t="s">
-        <v>121</v>
+        <v>122</v>
       </c>
       <c r="C15" s="2"/>
     </row>
     <row r="16" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A16" s="2" t="s">
-        <v>122</v>
+        <v>123</v>
       </c>
       <c r="B16" s="2" t="s">
-        <v>123</v>
+        <v>124</v>
       </c>
       <c r="C16" s="2"/>
     </row>
     <row r="17" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A17" s="2" t="s">
-        <v>124</v>
+        <v>125</v>
       </c>
       <c r="B17" s="2" t="s">
-        <v>125</v>
+        <v>126</v>
       </c>
       <c r="C17" s="2"/>
     </row>
     <row r="18" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A18" s="2" t="s">
-        <v>124</v>
+        <v>125</v>
       </c>
       <c r="B18" s="2" t="s">
-        <v>125</v>
+        <v>126</v>
       </c>
       <c r="C18" s="2"/>
     </row>
@@ -3824,10 +3827,10 @@
   <sheetData>
     <row r="1" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A1" s="3" t="s">
-        <v>126</v>
+        <v>127</v>
       </c>
       <c r="B1" s="3" t="s">
-        <v>127</v>
+        <v>128</v>
       </c>
       <c r="C1" s="3" t="s">
         <v>2</v>
@@ -3836,505 +3839,505 @@
     </row>
     <row r="2" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A2" s="4" t="s">
-        <v>128</v>
+        <v>129</v>
       </c>
       <c r="B2" s="4" t="s">
-        <v>129</v>
+        <v>130</v>
       </c>
       <c r="C2" s="4" t="s">
-        <v>130</v>
+        <v>131</v>
       </c>
       <c r="D2" s="4"/>
     </row>
     <row r="3" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A3" s="4" t="s">
-        <v>131</v>
+        <v>132</v>
       </c>
       <c r="B3" s="4" t="s">
-        <v>129</v>
+        <v>130</v>
       </c>
       <c r="C3" s="4" t="s">
-        <v>132</v>
+        <v>133</v>
       </c>
       <c r="D3" s="4"/>
     </row>
     <row r="4" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A4" s="4" t="s">
-        <v>133</v>
+        <v>134</v>
       </c>
       <c r="B4" s="4" t="s">
-        <v>129</v>
+        <v>130</v>
       </c>
       <c r="C4" s="4" t="s">
-        <v>134</v>
+        <v>135</v>
       </c>
       <c r="D4" s="4"/>
     </row>
     <row r="5" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A5" s="4" t="s">
-        <v>135</v>
+        <v>136</v>
       </c>
       <c r="B5" s="4" t="s">
-        <v>129</v>
+        <v>130</v>
       </c>
       <c r="C5" s="4" t="s">
-        <v>136</v>
+        <v>137</v>
       </c>
       <c r="D5" s="4"/>
     </row>
     <row r="6" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A6" s="4" t="s">
-        <v>137</v>
+        <v>138</v>
       </c>
       <c r="B6" s="4" t="s">
-        <v>129</v>
+        <v>130</v>
       </c>
       <c r="C6" s="4" t="s">
-        <v>138</v>
+        <v>139</v>
       </c>
       <c r="D6" s="4"/>
     </row>
     <row r="7" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A7" s="4" t="s">
-        <v>139</v>
+        <v>140</v>
       </c>
       <c r="B7" s="4" t="s">
-        <v>129</v>
+        <v>130</v>
       </c>
       <c r="C7" s="4" t="s">
-        <v>140</v>
+        <v>141</v>
       </c>
       <c r="D7" s="4"/>
     </row>
     <row r="8" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A8" s="4" t="s">
-        <v>141</v>
+        <v>142</v>
       </c>
       <c r="B8" s="4" t="s">
-        <v>129</v>
+        <v>130</v>
       </c>
       <c r="C8" s="4" t="s">
-        <v>142</v>
+        <v>143</v>
       </c>
       <c r="D8" s="4"/>
     </row>
     <row r="9" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A9" s="4" t="s">
-        <v>143</v>
+        <v>144</v>
       </c>
       <c r="B9" s="4" t="s">
-        <v>144</v>
+        <v>145</v>
       </c>
       <c r="C9" s="4" t="s">
-        <v>145</v>
+        <v>146</v>
       </c>
       <c r="D9" s="4"/>
     </row>
     <row r="10" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A10" s="4" t="s">
-        <v>146</v>
+        <v>147</v>
       </c>
       <c r="B10" s="4" t="s">
-        <v>144</v>
+        <v>145</v>
       </c>
       <c r="C10" s="4" t="s">
-        <v>147</v>
+        <v>148</v>
       </c>
       <c r="D10" s="4"/>
     </row>
     <row r="11" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A11" s="4" t="s">
-        <v>148</v>
+        <v>149</v>
       </c>
       <c r="B11" s="4" t="s">
-        <v>144</v>
+        <v>145</v>
       </c>
       <c r="C11" s="4" t="s">
-        <v>149</v>
+        <v>150</v>
       </c>
       <c r="D11" s="4"/>
     </row>
     <row r="12" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A12" s="4" t="s">
-        <v>150</v>
+        <v>151</v>
       </c>
       <c r="B12" s="4" t="s">
-        <v>144</v>
+        <v>145</v>
       </c>
       <c r="C12" s="4" t="s">
-        <v>151</v>
+        <v>152</v>
       </c>
       <c r="D12" s="4"/>
     </row>
     <row r="13" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A13" s="4" t="s">
-        <v>152</v>
+        <v>153</v>
       </c>
       <c r="B13" s="4" t="s">
-        <v>144</v>
+        <v>145</v>
       </c>
       <c r="C13" s="4" t="s">
-        <v>153</v>
+        <v>154</v>
       </c>
       <c r="D13" s="4"/>
     </row>
     <row r="14" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A14" s="4" t="s">
-        <v>154</v>
+        <v>155</v>
       </c>
       <c r="B14" s="4" t="s">
-        <v>144</v>
+        <v>145</v>
       </c>
       <c r="C14" s="4" t="s">
-        <v>155</v>
+        <v>156</v>
       </c>
       <c r="D14" s="4"/>
     </row>
     <row r="15" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A15" s="4" t="s">
-        <v>156</v>
+        <v>157</v>
       </c>
       <c r="B15" s="4" t="s">
-        <v>144</v>
+        <v>145</v>
       </c>
       <c r="C15" s="4" t="s">
-        <v>157</v>
+        <v>158</v>
       </c>
       <c r="D15" s="4"/>
     </row>
     <row r="16" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A16" s="4" t="s">
-        <v>158</v>
+        <v>159</v>
       </c>
       <c r="B16" s="4" t="s">
-        <v>159</v>
+        <v>160</v>
       </c>
       <c r="C16" s="4" t="s">
-        <v>160</v>
+        <v>161</v>
       </c>
       <c r="D16" s="4"/>
     </row>
     <row r="17" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A17" s="4" t="s">
-        <v>161</v>
+        <v>162</v>
       </c>
       <c r="B17" s="4" t="s">
-        <v>159</v>
+        <v>160</v>
       </c>
       <c r="C17" s="4" t="s">
-        <v>162</v>
+        <v>163</v>
       </c>
       <c r="D17" s="4"/>
     </row>
     <row r="18" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A18" s="4" t="s">
-        <v>163</v>
+        <v>164</v>
       </c>
       <c r="B18" s="4" t="s">
-        <v>159</v>
+        <v>160</v>
       </c>
       <c r="C18" s="4" t="s">
-        <v>164</v>
+        <v>165</v>
       </c>
       <c r="D18" s="4"/>
     </row>
     <row r="19" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A19" s="4" t="s">
-        <v>165</v>
+        <v>166</v>
       </c>
       <c r="B19" s="4" t="s">
-        <v>159</v>
+        <v>160</v>
       </c>
       <c r="C19" s="4" t="s">
-        <v>166</v>
+        <v>167</v>
       </c>
       <c r="D19" s="4"/>
     </row>
     <row r="20" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A20" s="4" t="s">
-        <v>167</v>
+        <v>168</v>
       </c>
       <c r="B20" s="4" t="s">
-        <v>159</v>
+        <v>160</v>
       </c>
       <c r="C20" s="4" t="s">
-        <v>168</v>
+        <v>169</v>
       </c>
       <c r="D20" s="4"/>
     </row>
     <row r="21" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A21" s="4" t="s">
-        <v>169</v>
+        <v>170</v>
       </c>
       <c r="B21" s="4" t="s">
-        <v>159</v>
+        <v>160</v>
       </c>
       <c r="C21" s="4" t="s">
-        <v>170</v>
+        <v>171</v>
       </c>
       <c r="D21" s="4"/>
     </row>
     <row r="22" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A22" s="4" t="s">
-        <v>171</v>
+        <v>172</v>
       </c>
       <c r="B22" s="4" t="s">
-        <v>159</v>
+        <v>160</v>
       </c>
       <c r="C22" s="4" t="s">
-        <v>172</v>
+        <v>173</v>
       </c>
       <c r="D22" s="4"/>
     </row>
     <row r="23" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A23" s="4" t="s">
-        <v>173</v>
+        <v>174</v>
       </c>
       <c r="B23" s="4" t="s">
-        <v>174</v>
+        <v>175</v>
       </c>
       <c r="C23" s="4" t="s">
-        <v>175</v>
+        <v>176</v>
       </c>
       <c r="D23" s="4"/>
     </row>
     <row r="24" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A24" s="4" t="s">
-        <v>176</v>
+        <v>177</v>
       </c>
       <c r="B24" s="4" t="s">
-        <v>174</v>
+        <v>175</v>
       </c>
       <c r="C24" s="4" t="s">
-        <v>177</v>
+        <v>178</v>
       </c>
       <c r="D24" s="4"/>
     </row>
     <row r="25" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A25" s="4" t="s">
-        <v>178</v>
+        <v>179</v>
       </c>
       <c r="B25" s="4" t="s">
-        <v>174</v>
+        <v>175</v>
       </c>
       <c r="C25" s="4" t="s">
-        <v>179</v>
+        <v>180</v>
       </c>
       <c r="D25" s="4"/>
     </row>
     <row r="26" customFormat="false" ht="30" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A26" s="4" t="s">
-        <v>180</v>
+        <v>181</v>
       </c>
       <c r="B26" s="4" t="s">
-        <v>174</v>
+        <v>175</v>
       </c>
       <c r="C26" s="5" t="s">
-        <v>181</v>
+        <v>182</v>
       </c>
       <c r="D26" s="4"/>
     </row>
     <row r="27" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A27" s="4" t="s">
-        <v>182</v>
+        <v>183</v>
       </c>
       <c r="B27" s="4" t="s">
-        <v>174</v>
+        <v>175</v>
       </c>
       <c r="C27" s="4" t="s">
-        <v>183</v>
+        <v>184</v>
       </c>
       <c r="D27" s="4"/>
     </row>
     <row r="28" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A28" s="4" t="s">
-        <v>184</v>
+        <v>185</v>
       </c>
       <c r="B28" s="4" t="s">
-        <v>174</v>
+        <v>175</v>
       </c>
       <c r="C28" s="4" t="s">
-        <v>185</v>
+        <v>186</v>
       </c>
       <c r="D28" s="4"/>
     </row>
     <row r="29" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A29" s="4" t="s">
-        <v>186</v>
+        <v>187</v>
       </c>
       <c r="B29" s="4" t="s">
-        <v>174</v>
+        <v>175</v>
       </c>
       <c r="C29" s="4" t="s">
-        <v>187</v>
+        <v>188</v>
       </c>
       <c r="D29" s="4"/>
     </row>
     <row r="30" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A30" s="4" t="s">
-        <v>188</v>
+        <v>189</v>
       </c>
       <c r="B30" s="4" t="s">
-        <v>189</v>
+        <v>190</v>
       </c>
       <c r="C30" s="4" t="s">
-        <v>190</v>
+        <v>191</v>
       </c>
       <c r="D30" s="4"/>
     </row>
     <row r="31" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A31" s="4" t="s">
-        <v>191</v>
+        <v>192</v>
       </c>
       <c r="B31" s="4" t="s">
-        <v>189</v>
+        <v>190</v>
       </c>
       <c r="C31" s="4" t="s">
-        <v>192</v>
+        <v>193</v>
       </c>
       <c r="D31" s="4"/>
     </row>
     <row r="32" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A32" s="4" t="s">
-        <v>193</v>
+        <v>194</v>
       </c>
       <c r="B32" s="4" t="s">
-        <v>189</v>
+        <v>190</v>
       </c>
       <c r="C32" s="4" t="s">
-        <v>194</v>
+        <v>195</v>
       </c>
       <c r="D32" s="4"/>
     </row>
     <row r="33" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A33" s="4" t="s">
-        <v>195</v>
+        <v>196</v>
       </c>
       <c r="B33" s="4" t="s">
-        <v>189</v>
+        <v>190</v>
       </c>
       <c r="C33" s="4" t="s">
-        <v>196</v>
+        <v>197</v>
       </c>
       <c r="D33" s="4"/>
     </row>
     <row r="34" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A34" s="4" t="s">
-        <v>197</v>
+        <v>198</v>
       </c>
       <c r="B34" s="4" t="s">
-        <v>189</v>
+        <v>190</v>
       </c>
       <c r="C34" s="4" t="s">
-        <v>198</v>
+        <v>199</v>
       </c>
       <c r="D34" s="4"/>
     </row>
     <row r="35" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A35" s="4" t="s">
-        <v>199</v>
+        <v>200</v>
       </c>
       <c r="B35" s="4" t="s">
-        <v>189</v>
+        <v>190</v>
       </c>
       <c r="C35" s="4" t="s">
-        <v>200</v>
+        <v>201</v>
       </c>
       <c r="D35" s="4"/>
     </row>
     <row r="36" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A36" s="4" t="s">
-        <v>201</v>
+        <v>202</v>
       </c>
       <c r="B36" s="4" t="s">
-        <v>189</v>
+        <v>190</v>
       </c>
       <c r="C36" s="4" t="s">
-        <v>202</v>
+        <v>203</v>
       </c>
       <c r="D36" s="4"/>
     </row>
     <row r="37" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A37" s="4" t="s">
-        <v>203</v>
+        <v>204</v>
       </c>
       <c r="B37" s="4" t="s">
-        <v>204</v>
+        <v>205</v>
       </c>
       <c r="C37" s="4" t="s">
-        <v>205</v>
+        <v>206</v>
       </c>
       <c r="D37" s="4"/>
     </row>
     <row r="38" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A38" s="4" t="s">
-        <v>206</v>
+        <v>207</v>
       </c>
       <c r="B38" s="4" t="s">
-        <v>204</v>
+        <v>205</v>
       </c>
       <c r="C38" s="4" t="s">
-        <v>207</v>
+        <v>208</v>
       </c>
       <c r="D38" s="4"/>
     </row>
     <row r="39" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A39" s="4" t="s">
-        <v>208</v>
+        <v>209</v>
       </c>
       <c r="B39" s="4" t="s">
-        <v>204</v>
+        <v>205</v>
       </c>
       <c r="C39" s="4" t="s">
-        <v>209</v>
+        <v>210</v>
       </c>
       <c r="D39" s="4"/>
     </row>
     <row r="40" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A40" s="4" t="s">
-        <v>210</v>
+        <v>211</v>
       </c>
       <c r="B40" s="4" t="s">
-        <v>204</v>
+        <v>205</v>
       </c>
       <c r="C40" s="4" t="s">
-        <v>211</v>
+        <v>212</v>
       </c>
       <c r="D40" s="4"/>
     </row>
     <row r="41" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A41" s="4" t="s">
-        <v>212</v>
+        <v>213</v>
       </c>
       <c r="B41" s="4" t="s">
-        <v>204</v>
+        <v>205</v>
       </c>
       <c r="C41" s="4" t="s">
-        <v>213</v>
+        <v>214</v>
       </c>
       <c r="D41" s="4"/>
     </row>
     <row r="42" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A42" s="4" t="s">
-        <v>214</v>
+        <v>215</v>
       </c>
       <c r="B42" s="4" t="s">
-        <v>204</v>
+        <v>205</v>
       </c>
       <c r="C42" s="4" t="s">
-        <v>215</v>
+        <v>216</v>
       </c>
       <c r="D42" s="4"/>
     </row>
     <row r="43" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A43" s="4" t="s">
-        <v>216</v>
+        <v>217</v>
       </c>
       <c r="B43" s="4" t="s">
-        <v>204</v>
+        <v>205</v>
       </c>
       <c r="C43" s="4" t="s">
-        <v>217</v>
+        <v>218</v>
       </c>
       <c r="D43" s="4"/>
     </row>
@@ -4371,16 +4374,16 @@
   <sheetData>
     <row r="1" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A1" s="1" t="s">
-        <v>218</v>
+        <v>219</v>
       </c>
       <c r="B1" s="1" t="s">
-        <v>219</v>
+        <v>220</v>
       </c>
       <c r="C1" s="1" t="s">
-        <v>220</v>
+        <v>221</v>
       </c>
       <c r="D1" s="1" t="s">
-        <v>221</v>
+        <v>222</v>
       </c>
       <c r="E1" s="1"/>
     </row>
@@ -4624,16 +4627,16 @@
   <sheetData>
     <row r="1" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A1" s="1" t="s">
-        <v>222</v>
+        <v>223</v>
       </c>
       <c r="B1" s="1" t="s">
-        <v>223</v>
+        <v>224</v>
       </c>
       <c r="C1" s="1" t="s">
-        <v>224</v>
+        <v>225</v>
       </c>
       <c r="D1" s="1" t="s">
-        <v>225</v>
+        <v>226</v>
       </c>
       <c r="E1" s="1"/>
     </row>
@@ -4877,16 +4880,16 @@
   <sheetData>
     <row r="1" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A1" s="1" t="s">
-        <v>226</v>
+        <v>227</v>
       </c>
       <c r="B1" s="1" t="s">
-        <v>227</v>
+        <v>228</v>
       </c>
       <c r="C1" s="1" t="s">
-        <v>228</v>
+        <v>229</v>
       </c>
       <c r="D1" s="1" t="s">
-        <v>229</v>
+        <v>230</v>
       </c>
       <c r="E1" s="1"/>
     </row>
@@ -5130,7 +5133,7 @@
   <sheetData>
     <row r="1" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A1" s="1" t="s">
-        <v>230</v>
+        <v>231</v>
       </c>
       <c r="B1" s="1"/>
     </row>

</xml_diff>

<commit_message>
Updated excel with greek ability
</commit_message>
<xml_diff>
--- a/src/main/resources/assets/gamedata-faf-waw.xlsx
+++ b/src/main/resources/assets/gamedata-faf-waw.xlsx
@@ -5,7 +5,7 @@
   <workbookPr backupFile="false" showObjects="all" date1904="false"/>
   <workbookProtection/>
   <bookViews>
-    <workbookView showHorizontalScroll="true" showVerticalScroll="true" showSheetTabs="true" xWindow="0" yWindow="0" windowWidth="16384" windowHeight="8192" tabRatio="600" firstSheet="0" activeTab="2"/>
+    <workbookView showHorizontalScroll="true" showVerticalScroll="true" showSheetTabs="true" xWindow="0" yWindow="0" windowWidth="16384" windowHeight="8192" tabRatio="600" firstSheet="0" activeTab="0"/>
   </bookViews>
   <sheets>
     <sheet name="Civ" sheetId="1" state="visible" r:id="rId2"/>
@@ -122,7 +122,7 @@
     <t>Democracy</t>
   </si>
   <si>
-    <t>Each time the Greeks gain a great person, they draw one extra great person, keeping one and discarding the other.</t>
+    <t>Each time the Greeks gain a great person, they draw one extra great person, keeping one and discarding the other. After the Greeks research or learn a tech, gain 1 culture for each player who does not currently know or is researching that tech</t>
   </si>
   <si>
     <t>Indians</t>
@@ -1329,8 +1329,8 @@
   </sheetPr>
   <dimension ref="A1:C17"/>
   <sheetViews>
-    <sheetView windowProtection="false" showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A4" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="D47" activeCellId="0" sqref="D47"/>
+    <sheetView windowProtection="false" showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A4" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
+      <selection pane="topLeft" activeCell="C11" activeCellId="0" sqref="C11"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15"/>
@@ -3358,7 +3358,7 @@
   </sheetPr>
   <dimension ref="A1:C26"/>
   <sheetViews>
-    <sheetView windowProtection="false" showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
+    <sheetView windowProtection="false" showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
       <selection pane="topLeft" activeCell="A25" activeCellId="0" sqref="A25"/>
     </sheetView>
   </sheetViews>

</xml_diff>